<commit_message>
data file checker + nieuwe meting + betere logging bij metingen
</commit_message>
<xml_diff>
--- a/measurements/single-fold_single-iteration.xlsx
+++ b/measurements/single-fold_single-iteration.xlsx
@@ -2291,7 +2291,7 @@
   <dimension ref="A1:BC25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF23" sqref="AF23"/>
+      <selection activeCell="AJ9" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3887,6 +3887,7 @@
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="AJ15" s="8"/>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -3936,6 +3937,7 @@
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="AJ16" s="8"/>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -3985,6 +3987,7 @@
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="AJ17" s="8"/>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -4034,6 +4037,7 @@
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="AJ18" s="8"/>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -4083,6 +4087,7 @@
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="AJ19" s="8"/>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -4127,21 +4132,37 @@
         <f t="shared" si="17"/>
         <v>2447537</v>
       </c>
-      <c r="AD20" s="16" t="e">
+      <c r="AB20">
+        <v>532535</v>
+      </c>
+      <c r="AC20">
+        <v>879155</v>
+      </c>
+      <c r="AD20" s="16">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE20" s="16" t="e">
+        <v>2984.8015253282983</v>
+      </c>
+      <c r="AE20" s="16">
         <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG20" s="16" t="e">
+        <v>3.4749154579710915</v>
+      </c>
+      <c r="AF20">
+        <v>390158</v>
+      </c>
+      <c r="AG20" s="16">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH20" s="16" t="e">
+        <v>6725.7449161621698</v>
+      </c>
+      <c r="AH20" s="16">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>3.8277403920294728</v>
+      </c>
+      <c r="AI20">
+        <v>474783</v>
+      </c>
+      <c r="AJ20" s="8">
+        <f>SUM(AB20,AC20,AF20,AI20)</f>
+        <v>2276631</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
@@ -4187,21 +4208,37 @@
         <f t="shared" si="17"/>
         <v>5114205</v>
       </c>
-      <c r="AD21" s="16" t="e">
+      <c r="AB21">
+        <v>739182</v>
+      </c>
+      <c r="AC21">
+        <v>878337</v>
+      </c>
+      <c r="AD21" s="16">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE21" s="16" t="e">
+        <v>5252.3150351175009</v>
+      </c>
+      <c r="AE21" s="16">
         <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG21" s="16" t="e">
+        <v>3.7203507672860376</v>
+      </c>
+      <c r="AF21">
+        <v>462342</v>
+      </c>
+      <c r="AG21" s="16">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH21" s="16" t="e">
+        <v>9978.1171319066834</v>
+      </c>
+      <c r="AH21" s="16">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>3.9990485977633301</v>
+      </c>
+      <c r="AI21">
+        <v>335683</v>
+      </c>
+      <c r="AJ21" s="8">
+        <f>SUM(AB21,AC21,AF21,AI21)</f>
+        <v>2415544</v>
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
@@ -4247,7 +4284,7 @@
       <c r="AI22">
         <v>333875</v>
       </c>
-      <c r="AJ22">
+      <c r="AJ22" s="8">
         <v>8450489</v>
       </c>
     </row>
@@ -4264,6 +4301,7 @@
       </c>
       <c r="AA23" s="8"/>
       <c r="AG23" s="16"/>
+      <c r="AJ23" s="8"/>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" t="s">

</xml_diff>

<commit_message>
genoeg voor vandaag -> naar huis
</commit_message>
<xml_diff>
--- a/measurements/single-fold_single-iteration.xlsx
+++ b/measurements/single-fold_single-iteration.xlsx
@@ -80,9 +80,6 @@
     <t xml:space="preserve">    - MINI</t>
   </si>
   <si>
-    <t>Cluster (4 data nodes) (bonte salie)</t>
-  </si>
-  <si>
     <t>Cluster (1 data nodes) (avanade)</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>ListNet Improved</t>
+  </si>
+  <si>
+    <t>Cluster (4 data nodes) (bonte salie, 30k en c2 Avanade)</t>
   </si>
 </sst>
 </file>
@@ -629,10 +629,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$T$4:$T$9</c:f>
+              <c:f>Sheet1!$T$4:$T$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>499522</c:v>
                 </c:pt>
@@ -647,9 +647,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>594616</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1273523</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1991,16 +1988,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>33618</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>179295</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>112059</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>22413</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>179294</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>179294</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2287,8 +2284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH22" sqref="AH22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2340,7 +2337,7 @@
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
@@ -2348,7 +2345,7 @@
       <c r="H1" s="22"/>
       <c r="I1" s="23"/>
       <c r="J1" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
@@ -2359,7 +2356,7 @@
       <c r="Q1" s="22"/>
       <c r="R1" s="23"/>
       <c r="S1" s="21" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="T1" s="22"/>
       <c r="U1" s="22"/>
@@ -2370,7 +2367,7 @@
       <c r="Z1" s="22"/>
       <c r="AA1" s="23"/>
       <c r="AB1" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AC1" s="22"/>
       <c r="AD1" s="22"/>
@@ -2381,7 +2378,7 @@
       <c r="AI1" s="22"/>
       <c r="AJ1" s="23"/>
       <c r="AK1" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AL1" s="22"/>
       <c r="AM1" s="22"/>
@@ -2389,7 +2386,7 @@
       <c r="AO1" s="22"/>
       <c r="AP1" s="23"/>
       <c r="AQ1" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AR1" s="22"/>
       <c r="AS1" s="22"/>
@@ -2414,10 +2411,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>11</v>
@@ -2432,19 +2429,19 @@
         <v>10</v>
       </c>
       <c r="L2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="O2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>11</v>
@@ -2459,19 +2456,19 @@
         <v>10</v>
       </c>
       <c r="U2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="X2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y2" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="Z2" s="6" t="s">
         <v>11</v>
@@ -2486,19 +2483,19 @@
         <v>10</v>
       </c>
       <c r="AD2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AE2" s="9" t="s">
+      <c r="AF2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AF2" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="AG2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH2" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="AI2" s="9" t="s">
         <v>11</v>
@@ -2513,10 +2510,10 @@
         <v>10</v>
       </c>
       <c r="AM2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN2" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="AO2" t="s">
         <v>11</v>
@@ -2531,7 +2528,7 @@
         <v>10</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AT2" s="3"/>
       <c r="AU2" t="s">
@@ -2548,10 +2545,10 @@
         <v>10</v>
       </c>
       <c r="AZ2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BA2" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="BA2" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="BB2" t="s">
         <v>11</v>
@@ -2711,7 +2708,7 @@
         <v>0.71840505859776227</v>
       </c>
       <c r="AH4" s="16">
-        <f t="shared" ref="AH4:AH23" si="7">LOG(AG4)</f>
+        <f t="shared" ref="AH4:AH21" si="7">LOG(AG4)</f>
         <v>-0.14363061827649873</v>
       </c>
       <c r="AI4" s="16">
@@ -2828,7 +2825,7 @@
         <v>10.928945750434707</v>
       </c>
       <c r="V5" s="16">
-        <f t="shared" ref="V5:V21" si="10">LOG(U5)</f>
+        <f t="shared" ref="V5:V19" si="10">LOG(U5)</f>
         <v>1.0385782701975261</v>
       </c>
       <c r="W5" s="16">
@@ -3312,7 +3309,7 @@
         <v>1312.2075170639512</v>
       </c>
       <c r="AE8" s="16">
-        <f t="shared" ref="AE8:AE22" si="15">LOG(AD8)</f>
+        <f t="shared" ref="AE8:AE21" si="15">LOG(AD8)</f>
         <v>3.1180025213118792</v>
       </c>
       <c r="AF8" s="16">
@@ -3440,40 +3437,40 @@
       <c r="Q9" s="16">
         <v>1156579</v>
       </c>
-      <c r="R9" s="16">
+      <c r="R9" s="18">
         <v>3793550</v>
       </c>
-      <c r="S9" s="15">
-        <v>656462</v>
-      </c>
-      <c r="T9" s="16">
-        <v>1273523</v>
+      <c r="S9">
+        <v>508491</v>
+      </c>
+      <c r="T9">
+        <v>908608</v>
       </c>
       <c r="U9" s="16">
-        <f t="shared" si="1"/>
-        <v>2060.5071011673917</v>
+        <f>B20/T9</f>
+        <v>2888.047634403395</v>
       </c>
       <c r="V9" s="16">
-        <f t="shared" si="10"/>
-        <v>3.3139741155810629</v>
-      </c>
-      <c r="W9" s="16">
-        <v>557466</v>
+        <f>LOG(U9)</f>
+        <v>3.4606043520513197</v>
+      </c>
+      <c r="W9">
+        <v>480568</v>
       </c>
       <c r="X9" s="16">
-        <f t="shared" si="2"/>
-        <v>4707.1986183910767</v>
+        <f>B20/W9</f>
+        <v>5460.4201382530673</v>
       </c>
       <c r="Y9" s="16">
-        <f t="shared" si="3"/>
-        <v>3.6727625235777683</v>
-      </c>
-      <c r="Z9" s="16">
-        <v>378601</v>
+        <f>LOG(X9)</f>
+        <v>3.7372260596837039</v>
+      </c>
+      <c r="Z9">
+        <v>549870</v>
       </c>
       <c r="AA9" s="18">
-        <f t="shared" si="4"/>
-        <v>2866052</v>
+        <f>SUM(S9:T9,W9,Z9)</f>
+        <v>2447537</v>
       </c>
       <c r="AB9" s="17">
         <v>429846</v>
@@ -3594,18 +3591,38 @@
       <c r="O10" s="16"/>
       <c r="P10" s="16"/>
       <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="16"/>
+      <c r="R10" s="18"/>
+      <c r="S10">
+        <v>913125</v>
+      </c>
+      <c r="T10">
+        <v>3111911</v>
+      </c>
+      <c r="U10" s="16">
+        <f>B21/T10</f>
+        <v>1482.4661216210875</v>
+      </c>
+      <c r="V10" s="16">
+        <f>LOG(U10)</f>
+        <v>3.1709847773407627</v>
+      </c>
+      <c r="W10">
+        <v>889609</v>
+      </c>
+      <c r="X10" s="16">
+        <f>B21/W10</f>
+        <v>5185.7643425370024</v>
+      </c>
+      <c r="Y10" s="16">
+        <f>LOG(X10)</f>
+        <v>3.7148127771727855</v>
+      </c>
+      <c r="Z10">
+        <v>199560</v>
+      </c>
       <c r="AA10" s="18">
-        <f t="shared" ref="AA10:AA21" si="17">SUM(S10:T10,W10,Z10)</f>
-        <v>0</v>
+        <f>SUM(S10:T10,W10,Z10)</f>
+        <v>5114205</v>
       </c>
       <c r="AB10" s="16">
         <v>515983</v>
@@ -3652,7 +3669,7 @@
       <c r="AU10" s="19"/>
       <c r="AV10" s="16"/>
       <c r="AX10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.25">
@@ -3690,30 +3707,41 @@
       <c r="Y11" s="16"/>
       <c r="Z11" s="16"/>
       <c r="AA11" s="18">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="AA10:AA19" si="17">SUM(S11:T11,W11,Z11)</f>
         <v>0</v>
       </c>
-      <c r="AB11" s="16"/>
-      <c r="AC11" s="16"/>
-      <c r="AD11" s="16" t="e">
+      <c r="AB11">
+        <v>951354</v>
+      </c>
+      <c r="AC11">
+        <v>1575972</v>
+      </c>
+      <c r="AD11" s="16">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE11" s="16" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF11" s="16"/>
-      <c r="AG11" s="16" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH11" s="16" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI11" s="16"/>
-      <c r="AJ11" s="18"/>
+        <v>7321.5812926879407</v>
+      </c>
+      <c r="AE11" s="16">
+        <f>LOG(AD11)</f>
+        <v>3.8646048887800566</v>
+      </c>
+      <c r="AF11">
+        <v>789234</v>
+      </c>
+      <c r="AG11" s="16">
+        <f>B22/AF11</f>
+        <v>14620.007644120755</v>
+      </c>
+      <c r="AH11" s="16">
+        <f>LOG(AG11)</f>
+        <v>4.1649475996942487</v>
+      </c>
+      <c r="AI11">
+        <v>178227</v>
+      </c>
+      <c r="AJ11" s="8">
+        <f>SUM(AI11,AF11,AC11,AB11)</f>
+        <v>3494787</v>
+      </c>
       <c r="AK11" s="19"/>
       <c r="AL11" s="19"/>
       <c r="AM11" s="19"/>
@@ -3727,7 +3755,7 @@
       <c r="AU11" s="19"/>
       <c r="AV11" s="16"/>
       <c r="AX11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.25">
@@ -3802,7 +3830,7 @@
       <c r="AU12" s="19"/>
       <c r="AV12" s="16"/>
       <c r="AX12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.25">
@@ -3819,7 +3847,7 @@
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -3829,12 +3857,18 @@
       <c r="V14" s="16"/>
       <c r="X14" s="16"/>
       <c r="Y14" s="16"/>
+      <c r="Z14" s="6"/>
       <c r="AA14" s="16"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
       <c r="AD14" s="16"/>
       <c r="AE14" s="16"/>
       <c r="AF14" s="16"/>
       <c r="AG14" s="16"/>
       <c r="AH14" s="16"/>
+      <c r="AI14" s="6"/>
+      <c r="AJ14" s="6"/>
+      <c r="AK14" s="6"/>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3847,47 +3881,22 @@
         <f t="shared" ref="C15:C23" si="18">LOG(B15)</f>
         <v>5.156488576050017</v>
       </c>
-      <c r="U15" s="16" t="e">
-        <f t="shared" ref="U15:U21" si="19">B15/T15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V15" s="16" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X15" s="16" t="e">
-        <f t="shared" ref="X15:X21" si="20">B15/W15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y15" s="16" t="e">
-        <f t="shared" ref="Y15:Y21" si="21">LOG(X15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA15" s="18">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AD15" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE15" s="16" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="16"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="16"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="16"/>
+      <c r="AE15" s="16"/>
       <c r="AF15" s="16"/>
-      <c r="AG15" s="16" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH15" s="16" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ15" s="8">
-        <f t="shared" ref="AJ15:AJ19" si="22">SUM(AB15,AC15,AF15,AI15)</f>
-        <v>0</v>
-      </c>
+      <c r="AG15" s="16"/>
+      <c r="AH15" s="16"/>
+      <c r="AI15" s="6"/>
+      <c r="AJ15" s="6"/>
+      <c r="AK15" s="6"/>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -3900,49 +3909,24 @@
         <f t="shared" si="18"/>
         <v>6.6580597867748397</v>
       </c>
-      <c r="U16" s="16" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V16" s="16" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X16" s="16" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y16" s="16" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA16" s="18">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AD16" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE16" s="16" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="16"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="16"/>
+      <c r="AE16" s="16"/>
       <c r="AF16" s="16"/>
-      <c r="AG16" s="16" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH16" s="16" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ16" s="8">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
+      <c r="AG16" s="16"/>
+      <c r="AH16" s="16"/>
+      <c r="AI16" s="6"/>
+      <c r="AJ16" s="6"/>
+      <c r="AK16" s="6"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -3953,49 +3937,24 @@
         <f t="shared" si="18"/>
         <v>6.7728354401561059</v>
       </c>
-      <c r="U17" s="16" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V17" s="16" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X17" s="16" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y17" s="16" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA17" s="18">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AD17" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE17" s="16" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="16"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="16"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="16"/>
+      <c r="AE17" s="16"/>
       <c r="AF17" s="16"/>
-      <c r="AG17" s="16" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH17" s="16" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ17" s="8">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
+      <c r="AG17" s="16"/>
+      <c r="AH17" s="16"/>
+      <c r="AI17" s="6"/>
+      <c r="AJ17" s="6"/>
+      <c r="AK17" s="6"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -4006,49 +3965,24 @@
         <f t="shared" si="18"/>
         <v>7.4119716953094192</v>
       </c>
-      <c r="U18" s="16" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V18" s="16" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X18" s="16" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y18" s="16" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA18" s="18">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AD18" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE18" s="16" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+      <c r="X18" s="16"/>
+      <c r="Y18" s="16"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="16"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="16"/>
+      <c r="AE18" s="16"/>
       <c r="AF18" s="16"/>
-      <c r="AG18" s="16" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH18" s="16" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ18" s="8">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
+      <c r="AG18" s="16"/>
+      <c r="AH18" s="16"/>
+      <c r="AI18" s="6"/>
+      <c r="AJ18" s="6"/>
+      <c r="AK18" s="6"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -4059,49 +3993,24 @@
         <f t="shared" si="18"/>
         <v>8.9232497970923994</v>
       </c>
-      <c r="U19" s="16" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V19" s="16" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X19" s="16" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y19" s="16" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA19" s="18">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AD19" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE19" s="16" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
+      <c r="X19" s="16"/>
+      <c r="Y19" s="16"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="16"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="16"/>
+      <c r="AE19" s="16"/>
       <c r="AF19" s="16"/>
-      <c r="AG19" s="16" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH19" s="16" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ19" s="8">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
+      <c r="AG19" s="16"/>
+      <c r="AH19" s="16"/>
+      <c r="AI19" s="6"/>
+      <c r="AJ19" s="6"/>
+      <c r="AK19" s="6"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -4112,48 +4021,20 @@
         <f t="shared" si="18"/>
         <v>9.4189809083694165</v>
       </c>
-      <c r="U20" s="16" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V20" s="16" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X20" s="16" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y20" s="16" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA20" s="18">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AD20" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE20" s="16" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG20" s="16" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH20" s="16" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ20" s="8">
-        <f>SUM(AB20,AC20,AF20,AI20)</f>
-        <v>0</v>
-      </c>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="16"/>
+      <c r="AE20" s="16"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="16"/>
+      <c r="AH20" s="16"/>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="6"/>
+      <c r="AK20" s="6"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -4164,48 +4045,20 @@
         <f t="shared" si="18"/>
         <v>9.664011945105198</v>
       </c>
-      <c r="U21" s="16" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V21" s="16" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X21" s="16" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y21" s="16" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA21" s="18">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AD21" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE21" s="16" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG21" s="16" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH21" s="16" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ21" s="8">
-        <f>SUM(AB21,AC21,AF21,AI21)</f>
-        <v>0</v>
-      </c>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="16"/>
+      <c r="AE21" s="16"/>
+      <c r="AF21" s="6"/>
+      <c r="AG21" s="16"/>
+      <c r="AH21" s="16"/>
+      <c r="AI21" s="6"/>
+      <c r="AJ21" s="6"/>
+      <c r="AK21" s="6"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -4216,41 +4069,20 @@
         <f t="shared" si="18"/>
         <v>10.062153385973239</v>
       </c>
-      <c r="AA22" s="8"/>
-      <c r="AB22">
-        <v>951354</v>
-      </c>
-      <c r="AC22">
-        <v>1575972</v>
-      </c>
-      <c r="AD22" s="16">
-        <f>B22/AC22</f>
-        <v>7321.5812926879407</v>
-      </c>
-      <c r="AE22" s="16">
-        <f t="shared" si="15"/>
-        <v>3.8646048887800566</v>
-      </c>
-      <c r="AF22">
-        <v>789234</v>
-      </c>
-      <c r="AG22" s="16">
-        <f>B22/AF22</f>
-        <v>14620.007644120755</v>
-      </c>
-      <c r="AH22" s="16">
-        <f t="shared" si="7"/>
-        <v>4.1649475996942487</v>
-      </c>
-      <c r="AI22">
-        <v>178227</v>
-      </c>
-      <c r="AJ22" s="8">
-        <f>SUM(AI22,AF22,AC22,AB22)</f>
-        <v>3494787</v>
-      </c>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="6"/>
+      <c r="AD22" s="6"/>
+      <c r="AE22" s="6"/>
+      <c r="AF22" s="6"/>
+      <c r="AG22" s="6"/>
+      <c r="AH22" s="6"/>
+      <c r="AI22" s="6"/>
+      <c r="AJ22" s="6"/>
+      <c r="AK22" s="6"/>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -4261,12 +4093,34 @@
         <f t="shared" si="18"/>
         <v>10.363332945802444</v>
       </c>
-      <c r="AA23" s="8"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="6"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
       <c r="AG23" s="16"/>
       <c r="AH23" s="17"/>
-      <c r="AJ23" s="8"/>
+      <c r="AI23" s="6"/>
+      <c r="AJ23" s="6"/>
+      <c r="AK23" s="6"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="6"/>
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="6"/>
+      <c r="AG24" s="6"/>
+      <c r="AH24" s="6"/>
+      <c r="AI24" s="6"/>
+      <c r="AJ24" s="6"/>
+      <c r="AK24" s="6"/>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
patch ListNetCluster voor compatibility met modulaire datasets
</commit_message>
<xml_diff>
--- a/measurements/single-fold_single-iteration.xlsx
+++ b/measurements/single-fold_single-iteration.xlsx
@@ -1153,11 +1153,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="299825784"/>
-        <c:axId val="299830488"/>
+        <c:axId val="302382984"/>
+        <c:axId val="302383376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="299825784"/>
+        <c:axId val="302382984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1251,12 +1251,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299830488"/>
+        <c:crossAx val="302383376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="299830488"/>
+        <c:axId val="302383376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1351,7 +1351,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299825784"/>
+        <c:crossAx val="302382984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2284,8 +2284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2661,7 +2661,7 @@
         <v>499522</v>
       </c>
       <c r="U4" s="16">
-        <f t="shared" ref="U4:U9" si="1">B4/T4</f>
+        <f t="shared" ref="U4:U8" si="1">B4/T4</f>
         <v>0.28703440489107584</v>
       </c>
       <c r="V4" s="16">
@@ -2672,18 +2672,18 @@
         <v>195261</v>
       </c>
       <c r="X4" s="16">
-        <f t="shared" ref="X4:X9" si="2">B4/W4</f>
+        <f t="shared" ref="X4:X8" si="2">B4/W4</f>
         <v>0.73429922001833448</v>
       </c>
       <c r="Y4" s="16">
-        <f t="shared" ref="Y4:Y9" si="3">LOG(X4)</f>
+        <f t="shared" ref="Y4:Y8" si="3">LOG(X4)</f>
         <v>-0.13412693310488208</v>
       </c>
       <c r="Z4" s="16">
         <v>338429</v>
       </c>
       <c r="AA4" s="18">
-        <f t="shared" ref="AA4:AA9" si="4">SUM(S4:T4,W4,Z4)</f>
+        <f t="shared" ref="AA4:AA8" si="4">SUM(S4:T4,W4,Z4)</f>
         <v>1493443</v>
       </c>
       <c r="AB4" s="16">
@@ -2693,7 +2693,7 @@
         <v>569045</v>
       </c>
       <c r="AD4" s="16">
-        <f t="shared" ref="AD4:AD21" si="5">B4/AC4</f>
+        <f t="shared" ref="AD4:AD12" si="5">B4/AC4</f>
         <v>0.25196601323269691</v>
       </c>
       <c r="AE4" s="16">
@@ -2704,11 +2704,11 @@
         <v>199581</v>
       </c>
       <c r="AG4" s="16">
-        <f t="shared" ref="AG4:AG21" si="6">B4/AF4</f>
+        <f t="shared" ref="AG4:AG12" si="6">B4/AF4</f>
         <v>0.71840505859776227</v>
       </c>
       <c r="AH4" s="16">
-        <f t="shared" ref="AH4:AH21" si="7">LOG(AG4)</f>
+        <f t="shared" ref="AH4:AH12" si="7">LOG(AG4)</f>
         <v>-0.14363061827649873</v>
       </c>
       <c r="AI4" s="16">
@@ -2825,7 +2825,7 @@
         <v>10.928945750434707</v>
       </c>
       <c r="V5" s="16">
-        <f t="shared" ref="V5:V19" si="10">LOG(U5)</f>
+        <f t="shared" ref="V5:V8" si="10">LOG(U5)</f>
         <v>1.0385782701975261</v>
       </c>
       <c r="W5" s="16">
@@ -3309,7 +3309,7 @@
         <v>1312.2075170639512</v>
       </c>
       <c r="AE8" s="16">
-        <f t="shared" ref="AE8:AE21" si="15">LOG(AD8)</f>
+        <f t="shared" ref="AE8:AE12" si="15">LOG(AD8)</f>
         <v>3.1180025213118792</v>
       </c>
       <c r="AF8" s="16">
@@ -3707,7 +3707,7 @@
       <c r="Y11" s="16"/>
       <c r="Z11" s="16"/>
       <c r="AA11" s="18">
-        <f t="shared" ref="AA10:AA19" si="17">SUM(S11:T11,W11,Z11)</f>
+        <f t="shared" ref="AA11:AA12" si="17">SUM(S11:T11,W11,Z11)</f>
         <v>0</v>
       </c>
       <c r="AB11">

</xml_diff>

<commit_message>
begin ECIR-versie paper + betere benaming datachunks
</commit_message>
<xml_diff>
--- a/measurements/single-fold_single-iteration.xlsx
+++ b/measurements/single-fold_single-iteration.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="30">
   <si>
     <t>ListNet</t>
   </si>
@@ -112,6 +113,9 @@
   <si>
     <t>Cluster (4 data nodes) (bonte salie, 30k en c2 Avanade)</t>
   </si>
+  <si>
+    <t xml:space="preserve">    - CUSTOM-20</t>
+  </si>
 </sst>
 </file>
 
@@ -142,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -234,11 +238,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,6 +327,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,7 +392,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="nl-NL" baseline="0"/>
-              <a:t> training time</a:t>
+              <a:t> training time old</a:t>
             </a:r>
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
@@ -500,7 +531,7 @@
                   <c:v>9.4189809083694165</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.664011945105198</c:v>
+                  <c:v>9.7200109040333977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -622,7 +653,7 @@
                   <c:v>9.4189809083694165</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.664011945105198</c:v>
+                  <c:v>9.7200109040333977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -744,7 +775,7 @@
                   <c:v>9.4189809083694165</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.664011945105198</c:v>
+                  <c:v>9.7200109040333977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -872,7 +903,7 @@
                   <c:v>9.4189809083694165</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.664011945105198</c:v>
+                  <c:v>9.7200109040333977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -988,13 +1019,13 @@
                   <c:v>9.4189809083694165</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.664011945105198</c:v>
+                  <c:v>9.7200109040333977</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.062153385973239</c:v>
+                  <c:v>10.117950912705435</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.363332945802444</c:v>
+                  <c:v>10.418980908369416</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1153,11 +1184,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="302382984"/>
-        <c:axId val="302383376"/>
+        <c:axId val="317273000"/>
+        <c:axId val="317274568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="302382984"/>
+        <c:axId val="317273000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1251,12 +1282,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302383376"/>
+        <c:crossAx val="317274568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="302383376"/>
+        <c:axId val="317274568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1351,7 +1382,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302382984"/>
+        <c:crossAx val="317273000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1365,6 +1396,890 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>ListNet</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nl-NL" baseline="0"/>
+              <a:t> training time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4 data nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>143380</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4550507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5927007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25820919</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>838011150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2624103185</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5248206370</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13120515925</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26241031850</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52482063700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$W$4:$W$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>195261</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>172251</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>173947</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>195808</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>291619</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>480568</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>751593</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1037886</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1715801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>8 data nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>143380</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4550507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5927007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25820919</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>838011150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2624103185</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5248206370</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13120515925</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26241031850</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52482063700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AF$4:$AF$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>199581</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190076</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>170982</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>199027</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>273056</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>390642</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>508702</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>789234</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>956912</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1955530</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>ranklib</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>143380</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4550507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5927007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25820919</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>838011150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2624103185</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5248206370</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13120515925</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26241031850</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52482063700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AY$4:$AY$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4526</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14309</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="318580960"/>
+        <c:axId val="318582920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="318580960"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="100000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Data size</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-NL" baseline="0"/>
+                  <a:t> in Bytes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="318582920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="318582920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2000000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Running</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-NL" baseline="0"/>
+                  <a:t> time in thousands of seconds</a:t>
+                </a:r>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="318580960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1482,6 +2397,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
@@ -1984,25 +2939,529 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>112059</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>22413</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>268941</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2011,6 +3470,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2282,10 +3773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC25"/>
+  <dimension ref="A1:BC26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2608,7 +4099,7 @@
         <v>143380</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C12" si="0">LOG(B4)</f>
+        <f>LOG(B4)</f>
         <v>5.156488576050017</v>
       </c>
       <c r="D4" s="15">
@@ -2661,7 +4152,7 @@
         <v>499522</v>
       </c>
       <c r="U4" s="16">
-        <f t="shared" ref="U4:U8" si="1">B4/T4</f>
+        <f>B4/T4</f>
         <v>0.28703440489107584</v>
       </c>
       <c r="V4" s="16">
@@ -2672,18 +4163,18 @@
         <v>195261</v>
       </c>
       <c r="X4" s="16">
-        <f t="shared" ref="X4:X8" si="2">B4/W4</f>
+        <f>B4/W4</f>
         <v>0.73429922001833448</v>
       </c>
       <c r="Y4" s="16">
-        <f t="shared" ref="Y4:Y8" si="3">LOG(X4)</f>
+        <f t="shared" ref="Y4:Y8" si="0">LOG(X4)</f>
         <v>-0.13412693310488208</v>
       </c>
       <c r="Z4" s="16">
         <v>338429</v>
       </c>
       <c r="AA4" s="18">
-        <f t="shared" ref="AA4:AA8" si="4">SUM(S4:T4,W4,Z4)</f>
+        <f t="shared" ref="AA4:AA8" si="1">SUM(S4:T4,W4,Z4)</f>
         <v>1493443</v>
       </c>
       <c r="AB4" s="16">
@@ -2693,7 +4184,7 @@
         <v>569045</v>
       </c>
       <c r="AD4" s="16">
-        <f t="shared" ref="AD4:AD12" si="5">B4/AC4</f>
+        <f>B4/AC4</f>
         <v>0.25196601323269691</v>
       </c>
       <c r="AE4" s="16">
@@ -2704,11 +4195,11 @@
         <v>199581</v>
       </c>
       <c r="AG4" s="16">
-        <f t="shared" ref="AG4:AG12" si="6">B4/AF4</f>
+        <f>B4/AF4</f>
         <v>0.71840505859776227</v>
       </c>
       <c r="AH4" s="16">
-        <f t="shared" ref="AH4:AH12" si="7">LOG(AG4)</f>
+        <f t="shared" ref="AH4:AH13" si="2">LOG(AG4)</f>
         <v>-0.14363061827649873</v>
       </c>
       <c r="AI4" s="16">
@@ -2737,7 +4228,7 @@
         <v>37</v>
       </c>
       <c r="AZ4">
-        <f t="shared" ref="AZ4:AZ9" si="8">B4/AY4</f>
+        <f>B4/AY4</f>
         <v>3875.135135135135</v>
       </c>
       <c r="BA4">
@@ -2760,7 +4251,7 @@
         <v>4550507</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f>LOG(B5)</f>
         <v>6.6580597867748397</v>
       </c>
       <c r="D5" s="15">
@@ -2774,7 +4265,7 @@
         <v>13.617463723228207</v>
       </c>
       <c r="G5" s="16">
-        <f t="shared" ref="G5:G8" si="9">LOG(F5)</f>
+        <f t="shared" ref="G5:G8" si="3">LOG(F5)</f>
         <v>1.1340962269910448</v>
       </c>
       <c r="H5" s="17">
@@ -2821,29 +4312,29 @@
         <v>416372</v>
       </c>
       <c r="U5" s="16">
-        <f t="shared" si="1"/>
+        <f>B5/T5</f>
         <v>10.928945750434707</v>
       </c>
       <c r="V5" s="16">
-        <f t="shared" ref="V5:V8" si="10">LOG(U5)</f>
+        <f t="shared" ref="V5:V8" si="4">LOG(U5)</f>
         <v>1.0385782701975261</v>
       </c>
       <c r="W5" s="16">
         <v>172251</v>
       </c>
       <c r="X5" s="16">
-        <f t="shared" si="2"/>
+        <f>B5/W5</f>
         <v>26.417884366418772</v>
       </c>
       <c r="Y5" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1.4218980348992616</v>
       </c>
       <c r="Z5" s="16">
         <v>333838</v>
       </c>
       <c r="AA5" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1390684</v>
       </c>
       <c r="AB5" s="16">
@@ -2853,7 +4344,7 @@
         <v>545427</v>
       </c>
       <c r="AD5" s="16">
-        <f t="shared" si="5"/>
+        <f>B5/AC5</f>
         <v>8.3430174890498634</v>
       </c>
       <c r="AE5" s="16">
@@ -2864,11 +4355,11 @@
         <v>190076</v>
       </c>
       <c r="AG5" s="16">
-        <f t="shared" si="6"/>
+        <f>B5/AF5</f>
         <v>23.940460657842127</v>
       </c>
       <c r="AH5" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>1.3791325027635455</v>
       </c>
       <c r="AI5" s="16">
@@ -2898,18 +4389,18 @@
         <v>109</v>
       </c>
       <c r="AZ5">
-        <f t="shared" si="8"/>
+        <f>B5/AY5</f>
         <v>41747.770642201838</v>
       </c>
       <c r="BA5">
-        <f t="shared" ref="BA5:BA9" si="11">LOG(AZ5)</f>
+        <f t="shared" ref="BA5:BA9" si="5">LOG(AZ5)</f>
         <v>4.6206332888342159</v>
       </c>
       <c r="BB5">
         <v>4</v>
       </c>
       <c r="BC5">
-        <f t="shared" ref="BC5:BC8" si="12">SUM(AX5:BB5)</f>
+        <f t="shared" ref="BC5:BC8" si="6">SUM(AX5:BB5)</f>
         <v>42101.391275490671</v>
       </c>
     </row>
@@ -2921,7 +4412,7 @@
         <v>5927007</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f>LOG(B6)</f>
         <v>6.7728354401561059</v>
       </c>
       <c r="D6" s="15">
@@ -2935,7 +4426,7 @@
         <v>17.928735854706929</v>
       </c>
       <c r="G6" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>1.2535496687769128</v>
       </c>
       <c r="H6" s="16">
@@ -2960,29 +4451,29 @@
         <v>458863</v>
       </c>
       <c r="U6" s="16">
-        <f t="shared" si="1"/>
+        <f>B6/T6</f>
         <v>12.916724599717126</v>
       </c>
       <c r="V6" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>1.1111523999895863</v>
       </c>
       <c r="W6" s="16">
         <v>173947</v>
       </c>
       <c r="X6" s="16">
-        <f t="shared" si="2"/>
+        <f>B6/W6</f>
         <v>34.073637372303061</v>
       </c>
       <c r="Y6" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1.5324184971252766</v>
       </c>
       <c r="Z6" s="16">
         <v>312704</v>
       </c>
       <c r="AA6" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1426040</v>
       </c>
       <c r="AB6" s="16">
@@ -2992,7 +4483,7 @@
         <v>617337</v>
       </c>
       <c r="AD6" s="16">
-        <f t="shared" si="5"/>
+        <f>B6/AC6</f>
         <v>9.6009262363992445</v>
       </c>
       <c r="AE6" s="16">
@@ -3003,11 +4494,11 @@
         <v>170982</v>
       </c>
       <c r="AG6" s="16">
-        <f t="shared" si="6"/>
+        <f>B6/AF6</f>
         <v>34.664508544759094</v>
       </c>
       <c r="AH6" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>1.5398850473788057</v>
       </c>
       <c r="AI6" s="16">
@@ -3037,18 +4528,18 @@
         <v>142</v>
       </c>
       <c r="AZ6">
-        <f t="shared" si="8"/>
+        <f>B6/AY6</f>
         <v>41739.485915492958</v>
       </c>
       <c r="BA6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>4.6205470957730492</v>
       </c>
       <c r="BB6">
         <v>4</v>
       </c>
       <c r="BC6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>42119.10646258873</v>
       </c>
     </row>
@@ -3060,7 +4551,7 @@
         <v>25820919</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>LOG(B7)</f>
         <v>7.4119716953094192</v>
       </c>
       <c r="D7" s="15">
@@ -3074,7 +4565,7 @@
         <v>81.560263055652953</v>
       </c>
       <c r="G7" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>1.9114786178348209</v>
       </c>
       <c r="H7" s="17">
@@ -3094,7 +4585,7 @@
         <v>73.581061672527483</v>
       </c>
       <c r="M7" s="17">
-        <f t="shared" ref="M7:M9" si="13">LOG(L7)</f>
+        <f t="shared" ref="M7:M9" si="7">LOG(L7)</f>
         <v>1.8667660498065228</v>
       </c>
       <c r="N7" s="16">
@@ -3105,7 +4596,7 @@
         <v>130.94768364733625</v>
       </c>
       <c r="P7" s="17">
-        <f t="shared" ref="P7:P9" si="14">LOG(O7)</f>
+        <f t="shared" ref="P7:P9" si="8">LOG(O7)</f>
         <v>2.1170978205308009</v>
       </c>
       <c r="Q7" s="16">
@@ -3121,29 +4612,29 @@
         <v>393560</v>
       </c>
       <c r="U7" s="16">
-        <f t="shared" si="1"/>
+        <f>B7/T7</f>
         <v>65.60859589389166</v>
       </c>
       <c r="V7" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>1.8169607434110107</v>
       </c>
       <c r="W7" s="16">
         <v>195808</v>
       </c>
       <c r="X7" s="16">
-        <f t="shared" si="2"/>
+        <f>B7/W7</f>
         <v>131.86856001797679</v>
       </c>
       <c r="Y7" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>2.1201412637928647</v>
       </c>
       <c r="Z7" s="16">
         <v>167525</v>
       </c>
       <c r="AA7" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1251912</v>
       </c>
       <c r="AB7" s="16">
@@ -3153,7 +4644,7 @@
         <v>564471</v>
       </c>
       <c r="AD7" s="16">
-        <f t="shared" si="5"/>
+        <f>B7/AC7</f>
         <v>45.743570528866847</v>
       </c>
       <c r="AE7" s="16">
@@ -3164,11 +4655,11 @@
         <v>199027</v>
       </c>
       <c r="AG7" s="16">
-        <f t="shared" si="6"/>
+        <f>B7/AF7</f>
         <v>129.73575946982066</v>
       </c>
       <c r="AH7" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>2.113059698519792</v>
       </c>
       <c r="AI7" s="16">
@@ -3211,18 +4702,18 @@
         <v>211</v>
       </c>
       <c r="AZ7">
-        <f t="shared" si="8"/>
+        <f>B7/AY7</f>
         <v>122374.02369668246</v>
       </c>
       <c r="BA7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>5.0876892400117271</v>
       </c>
       <c r="BB7">
         <v>7</v>
       </c>
       <c r="BC7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>123354.11138592247</v>
       </c>
     </row>
@@ -3234,7 +4725,7 @@
         <v>838011150</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>LOG(B8)</f>
         <v>8.9232497970923994</v>
       </c>
       <c r="D8" s="15">
@@ -3248,7 +4739,7 @@
         <v>935.62907378420084</v>
       </c>
       <c r="G8" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>2.9711037086350469</v>
       </c>
       <c r="H8" s="17">
@@ -3273,29 +4764,29 @@
         <v>594616</v>
       </c>
       <c r="U8" s="16">
-        <f t="shared" si="1"/>
+        <f>B8/T8</f>
         <v>1409.3316526968665</v>
       </c>
       <c r="V8" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>3.1490132060172549</v>
       </c>
       <c r="W8" s="16">
         <v>291619</v>
       </c>
       <c r="X8" s="16">
-        <f t="shared" si="2"/>
+        <f>B8/W8</f>
         <v>2873.6507223466233</v>
       </c>
       <c r="Y8" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>3.4584339807169</v>
       </c>
       <c r="Z8" s="16">
         <v>365325</v>
       </c>
       <c r="AA8" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1687282</v>
       </c>
       <c r="AB8" s="16">
@@ -3305,22 +4796,22 @@
         <v>638627</v>
       </c>
       <c r="AD8" s="16">
-        <f t="shared" si="5"/>
+        <f>B8/AC8</f>
         <v>1312.2075170639512</v>
       </c>
       <c r="AE8" s="16">
-        <f t="shared" ref="AE8:AE12" si="15">LOG(AD8)</f>
+        <f t="shared" ref="AE8:AE13" si="9">LOG(AD8)</f>
         <v>3.1180025213118792</v>
       </c>
       <c r="AF8" s="16">
         <v>273056</v>
       </c>
       <c r="AG8" s="16">
-        <f t="shared" si="6"/>
+        <f>B8/AF8</f>
         <v>3069.008371909059</v>
       </c>
       <c r="AH8" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>3.486998073139854</v>
       </c>
       <c r="AI8" s="16">
@@ -3341,7 +4832,7 @@
         <v>1175.8935900620072</v>
       </c>
       <c r="AN8" s="17">
-        <f t="shared" ref="AN8:AN9" si="16">LOG(AM8)</f>
+        <f t="shared" ref="AN8:AN9" si="10">LOG(AM8)</f>
         <v>3.0703680229817771</v>
       </c>
       <c r="AO8" s="17">
@@ -3377,18 +4868,18 @@
         <v>4526</v>
       </c>
       <c r="AZ8">
-        <f t="shared" si="8"/>
+        <f>B8/AY8</f>
         <v>185154.916040654</v>
       </c>
       <c r="BA8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>5.2675352474736892</v>
       </c>
       <c r="BB8" s="17">
         <v>255</v>
       </c>
       <c r="BC8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>217883.18357590146</v>
       </c>
     </row>
@@ -3400,7 +4891,7 @@
         <v>2624103185</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>LOG(B9)</f>
         <v>9.4189809083694165</v>
       </c>
       <c r="D9" s="15"/>
@@ -3420,7 +4911,7 @@
         <v>1430.5684677818556</v>
       </c>
       <c r="M9" s="17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>3.1555086482078778</v>
       </c>
       <c r="N9" s="16">
@@ -3431,7 +4922,7 @@
         <v>3555.4833925890598</v>
       </c>
       <c r="P9" s="17">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>3.5508986544222787</v>
       </c>
       <c r="Q9" s="16">
@@ -3447,7 +4938,7 @@
         <v>908608</v>
       </c>
       <c r="U9" s="16">
-        <f>B20/T9</f>
+        <f>B21/T9</f>
         <v>2888.047634403395</v>
       </c>
       <c r="V9" s="16">
@@ -3458,7 +4949,7 @@
         <v>480568</v>
       </c>
       <c r="X9" s="16">
-        <f>B20/W9</f>
+        <f>B21/W9</f>
         <v>5460.4201382530673</v>
       </c>
       <c r="Y9" s="16">
@@ -3479,22 +4970,22 @@
         <v>914035</v>
       </c>
       <c r="AD9" s="16">
-        <f t="shared" si="5"/>
+        <f>B9/AC9</f>
         <v>2870.9001132341759</v>
       </c>
       <c r="AE9" s="16">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>3.4580180824213178</v>
       </c>
       <c r="AF9" s="16">
         <v>390642</v>
       </c>
       <c r="AG9" s="16">
-        <f t="shared" si="6"/>
+        <f>B9/AF9</f>
         <v>6717.4118118379492</v>
       </c>
       <c r="AH9" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>3.8272019735966758</v>
       </c>
       <c r="AI9" s="16">
@@ -3515,7 +5006,7 @@
         <v>3116.0050977453789</v>
       </c>
       <c r="AN9" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>3.4935981595014503</v>
       </c>
       <c r="AO9" s="17">
@@ -3551,11 +5042,11 @@
         <v>14309</v>
       </c>
       <c r="AZ9">
-        <f t="shared" si="8"/>
+        <f>B9/AY9</f>
         <v>183388.30002096583</v>
       </c>
       <c r="BA9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>5.2633716246905005</v>
       </c>
       <c r="BB9" s="17">
@@ -3571,11 +5062,12 @@
         <v>6</v>
       </c>
       <c r="B10" s="20">
-        <v>4613302631</v>
+        <f>2*B9</f>
+        <v>5248206370</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>9.664011945105198</v>
+        <f>LOG(B10)</f>
+        <v>9.7200109040333977</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
@@ -3593,36 +5085,36 @@
       <c r="Q10" s="16"/>
       <c r="R10" s="18"/>
       <c r="S10">
-        <v>913125</v>
+        <v>1097529</v>
       </c>
       <c r="T10">
-        <v>3111911</v>
+        <v>1514885</v>
       </c>
       <c r="U10" s="16">
-        <f>B21/T10</f>
-        <v>1482.4661216210875</v>
+        <f>B22/T10</f>
+        <v>3045.3154074401687</v>
       </c>
       <c r="V10" s="16">
         <f>LOG(U10)</f>
-        <v>3.1709847773407627</v>
+        <v>3.4836322797659336</v>
       </c>
       <c r="W10">
-        <v>889609</v>
+        <v>751593</v>
       </c>
       <c r="X10" s="16">
-        <f>B21/W10</f>
-        <v>5185.7643425370024</v>
+        <f>B22/W10</f>
+        <v>6138.0329925904043</v>
       </c>
       <c r="Y10" s="16">
         <f>LOG(X10)</f>
-        <v>3.7148127771727855</v>
+        <v>3.7880292184818329</v>
       </c>
       <c r="Z10">
-        <v>199560</v>
+        <v>368501</v>
       </c>
       <c r="AA10" s="18">
         <f>SUM(S10:T10,W10,Z10)</f>
-        <v>5114205</v>
+        <v>3732508</v>
       </c>
       <c r="AB10" s="16">
         <v>515983</v>
@@ -3631,23 +5123,23 @@
         <v>1076959</v>
       </c>
       <c r="AD10" s="16">
-        <f t="shared" si="5"/>
-        <v>4283.63812457113</v>
+        <f>B10/AC10</f>
+        <v>4873.1719313362901</v>
       </c>
       <c r="AE10" s="16">
-        <f t="shared" si="15"/>
-        <v>3.6318127751523366</v>
+        <f t="shared" si="9"/>
+        <v>3.687811734080535</v>
       </c>
       <c r="AF10" s="16">
         <v>508702</v>
       </c>
       <c r="AG10" s="16">
-        <f t="shared" si="6"/>
-        <v>9068.772348054461</v>
+        <f>B10/AF10</f>
+        <v>10316.858140915507</v>
       </c>
       <c r="AH10" s="16">
-        <f t="shared" si="7"/>
-        <v>3.9575485000092154</v>
+        <f t="shared" si="2"/>
+        <v>4.0135474589374143</v>
       </c>
       <c r="AI10" s="16">
         <v>338271</v>
@@ -3677,11 +5169,12 @@
         <v>7</v>
       </c>
       <c r="B11" s="20">
-        <v>11538607113</v>
+        <f>5*B9</f>
+        <v>13120515925</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>10.062153385973239</v>
+        <f>LOG(B11)</f>
+        <v>10.117950912705435</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="16"/>
@@ -3698,17 +5191,37 @@
       <c r="P11" s="16"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="16"/>
+      <c r="S11" s="15">
+        <v>1131941</v>
+      </c>
+      <c r="T11" s="16">
+        <v>1879565</v>
+      </c>
+      <c r="U11" s="16">
+        <f>B23/T11</f>
+        <v>6138.9774298840421</v>
+      </c>
+      <c r="V11" s="16">
+        <f>LOG(U11)</f>
+        <v>3.788096036687866</v>
+      </c>
+      <c r="W11" s="16">
+        <v>1037886</v>
+      </c>
+      <c r="X11" s="16">
+        <f>B23/W11</f>
+        <v>11117.412811233604</v>
+      </c>
+      <c r="Y11" s="16">
+        <f>LOG(X11)</f>
+        <v>4.0460037321620232</v>
+      </c>
+      <c r="Z11" s="16">
+        <v>363621</v>
+      </c>
       <c r="AA11" s="18">
-        <f t="shared" ref="AA11:AA12" si="17">SUM(S11:T11,W11,Z11)</f>
-        <v>0</v>
+        <f>SUM(S11:T11,W11,Z11)</f>
+        <v>4413013</v>
       </c>
       <c r="AB11">
         <v>951354</v>
@@ -3717,18 +5230,18 @@
         <v>1575972</v>
       </c>
       <c r="AD11" s="16">
-        <f t="shared" si="5"/>
-        <v>7321.5812926879407</v>
+        <f>B11/AC11</f>
+        <v>8325.3483723061072</v>
       </c>
       <c r="AE11" s="16">
         <f>LOG(AD11)</f>
-        <v>3.8646048887800566</v>
+        <v>3.9204024155122519</v>
       </c>
       <c r="AF11">
         <v>789234</v>
       </c>
       <c r="AG11" s="16">
-        <f>B22/AF11</f>
+        <f>B23/AF11</f>
         <v>14620.007644120755</v>
       </c>
       <c r="AH11" s="16">
@@ -3763,11 +5276,12 @@
         <v>8</v>
       </c>
       <c r="B12" s="20">
-        <v>23085163023</v>
+        <f>10*B9</f>
+        <v>26241031850</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>10.363332945802444</v>
+        <f>LOG(B12)</f>
+        <v>10.418980908369416</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="16"/>
@@ -3784,39 +5298,70 @@
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="16"/>
+      <c r="S12" s="15">
+        <v>1922426</v>
+      </c>
+      <c r="T12" s="16">
+        <v>3304425</v>
+      </c>
+      <c r="U12" s="16">
+        <f>B24/T12</f>
+        <v>6986.136172859121</v>
+      </c>
+      <c r="V12" s="16">
+        <f>LOG(U12)</f>
+        <v>3.844237046595778</v>
+      </c>
+      <c r="W12" s="16">
+        <v>1715801</v>
+      </c>
+      <c r="X12" s="16">
+        <f>B24/W12</f>
+        <v>13454.452481960321</v>
+      </c>
+      <c r="Y12" s="16">
+        <f>LOG(X12)</f>
+        <v>4.1288660291973933</v>
+      </c>
+      <c r="Z12" s="16">
+        <v>287681</v>
+      </c>
       <c r="AA12" s="18">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AB12" s="16"/>
-      <c r="AC12" s="16"/>
-      <c r="AD12" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE12" s="16" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF12" s="16"/>
-      <c r="AG12" s="16" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH12" s="16" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI12" s="16"/>
-      <c r="AJ12" s="18"/>
+        <f t="shared" ref="AA12" si="11">SUM(S12:T12,W12,Z12)</f>
+        <v>7230333</v>
+      </c>
+      <c r="AB12" s="16">
+        <v>1039155</v>
+      </c>
+      <c r="AC12" s="16">
+        <v>2037349</v>
+      </c>
+      <c r="AD12" s="16">
+        <f>B12/AC12</f>
+        <v>12879.988578294637</v>
+      </c>
+      <c r="AE12" s="16">
+        <f t="shared" si="9"/>
+        <v>4.109915477900671</v>
+      </c>
+      <c r="AF12" s="16">
+        <v>956912</v>
+      </c>
+      <c r="AG12" s="16">
+        <f>B12/AF12</f>
+        <v>27422.617597020417</v>
+      </c>
+      <c r="AH12" s="16">
+        <f t="shared" si="2"/>
+        <v>4.4381089075535556</v>
+      </c>
+      <c r="AI12" s="16">
+        <v>201019</v>
+      </c>
+      <c r="AJ12" s="8">
+        <f t="shared" ref="AJ12:AJ13" si="12">SUM(AI12,AF12,AC12,AB12)</f>
+        <v>4234435</v>
+      </c>
       <c r="AK12" s="19"/>
       <c r="AL12" s="19"/>
       <c r="AM12" s="19"/>
@@ -3834,53 +5379,78 @@
       </c>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="25">
+        <f>20*B9</f>
+        <v>52482063700</v>
+      </c>
+      <c r="C13" s="26">
+        <f>LOG(B13)</f>
+        <v>10.720010904033398</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="R13" s="8"/>
       <c r="U13" s="16"/>
       <c r="V13" s="16"/>
       <c r="X13" s="16"/>
       <c r="Y13" s="16"/>
-      <c r="AA13" s="16"/>
-      <c r="AD13" s="16"/>
-      <c r="AE13" s="16"/>
-      <c r="AF13" s="16"/>
-      <c r="AG13" s="16"/>
-      <c r="AH13" s="16"/>
+      <c r="AA13" s="18"/>
+      <c r="AB13" s="17">
+        <v>2319968</v>
+      </c>
+      <c r="AC13" s="17">
+        <v>3698960</v>
+      </c>
+      <c r="AD13" s="16">
+        <f>B13/AC13</f>
+        <v>14188.329611566494</v>
+      </c>
+      <c r="AE13" s="16">
+        <f t="shared" si="9"/>
+        <v>4.1519312690881582</v>
+      </c>
+      <c r="AF13" s="16">
+        <v>1955530</v>
+      </c>
+      <c r="AG13" s="16">
+        <f>B13/AF13</f>
+        <v>26837.769658353489</v>
+      </c>
+      <c r="AH13" s="16">
+        <f t="shared" si="2"/>
+        <v>4.4287464211349086</v>
+      </c>
+      <c r="AI13" s="17">
+        <v>199887</v>
+      </c>
+      <c r="AJ13" s="8">
+        <f t="shared" si="12"/>
+        <v>8174345</v>
+      </c>
+      <c r="AP13" s="8"/>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="8"/>
       <c r="U14" s="16"/>
       <c r="V14" s="16"/>
       <c r="X14" s="16"/>
       <c r="Y14" s="16"/>
-      <c r="Z14" s="6"/>
       <c r="AA14" s="16"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
       <c r="AD14" s="16"/>
       <c r="AE14" s="16"/>
       <c r="AF14" s="16"/>
       <c r="AG14" s="16"/>
       <c r="AH14" s="16"/>
-      <c r="AI14" s="6"/>
-      <c r="AJ14" s="6"/>
-      <c r="AK14" s="6"/>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>143380</v>
-      </c>
-      <c r="C15" s="8">
-        <f t="shared" ref="C15:C23" si="18">LOG(B15)</f>
-        <v>5.156488576050017</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="8"/>
       <c r="U15" s="16"/>
       <c r="V15" s="16"/>
       <c r="X15" s="16"/>
@@ -3900,14 +5470,14 @@
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>4550507</v>
+        <v>143380</v>
       </c>
       <c r="C16" s="8">
-        <f t="shared" si="18"/>
-        <v>6.6580597867748397</v>
+        <f t="shared" ref="C16:C24" si="13">LOG(B16)</f>
+        <v>5.156488576050017</v>
       </c>
       <c r="U16" s="16"/>
       <c r="V16" s="16"/>
@@ -3928,14 +5498,14 @@
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>5927007</v>
+        <v>4550507</v>
       </c>
       <c r="C17" s="8">
-        <f t="shared" si="18"/>
-        <v>6.7728354401561059</v>
+        <f t="shared" si="13"/>
+        <v>6.6580597867748397</v>
       </c>
       <c r="U17" s="16"/>
       <c r="V17" s="16"/>
@@ -3956,14 +5526,14 @@
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18">
-        <v>25820919</v>
+        <v>5927007</v>
       </c>
       <c r="C18" s="8">
-        <f t="shared" si="18"/>
-        <v>7.4119716953094192</v>
+        <f t="shared" si="13"/>
+        <v>6.7728354401561059</v>
       </c>
       <c r="U18" s="16"/>
       <c r="V18" s="16"/>
@@ -3984,14 +5554,14 @@
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B19">
-        <v>838011150</v>
+        <v>25820919</v>
       </c>
       <c r="C19" s="8">
-        <f t="shared" si="18"/>
-        <v>8.9232497970923994</v>
+        <f t="shared" si="13"/>
+        <v>7.4119716953094192</v>
       </c>
       <c r="U19" s="16"/>
       <c r="V19" s="16"/>
@@ -4012,22 +5582,26 @@
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20">
-        <v>2624103185</v>
+        <v>838011150</v>
       </c>
       <c r="C20" s="8">
-        <f t="shared" si="18"/>
-        <v>9.4189809083694165</v>
-      </c>
+        <f t="shared" si="13"/>
+        <v>8.9232497970923994</v>
+      </c>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="16"/>
       <c r="Z20" s="6"/>
-      <c r="AA20" s="6"/>
+      <c r="AA20" s="16"/>
       <c r="AB20" s="6"/>
       <c r="AC20" s="6"/>
       <c r="AD20" s="16"/>
       <c r="AE20" s="16"/>
-      <c r="AF20" s="6"/>
+      <c r="AF20" s="16"/>
       <c r="AG20" s="16"/>
       <c r="AH20" s="16"/>
       <c r="AI20" s="6"/>
@@ -4036,14 +5610,14 @@
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21">
-        <v>4613302631</v>
+        <v>2624103185</v>
       </c>
       <c r="C21" s="8">
-        <f t="shared" si="18"/>
-        <v>9.664011945105198</v>
+        <f t="shared" si="13"/>
+        <v>9.4189809083694165</v>
       </c>
       <c r="Z21" s="6"/>
       <c r="AA21" s="6"/>
@@ -4060,38 +5634,38 @@
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22">
-        <v>11538607113</v>
+        <v>4613302631</v>
       </c>
       <c r="C22" s="8">
-        <f t="shared" si="18"/>
-        <v>10.062153385973239</v>
+        <f t="shared" si="13"/>
+        <v>9.664011945105198</v>
       </c>
       <c r="Z22" s="6"/>
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
       <c r="AC22" s="6"/>
-      <c r="AD22" s="6"/>
-      <c r="AE22" s="6"/>
+      <c r="AD22" s="16"/>
+      <c r="AE22" s="16"/>
       <c r="AF22" s="6"/>
-      <c r="AG22" s="6"/>
-      <c r="AH22" s="6"/>
+      <c r="AG22" s="16"/>
+      <c r="AH22" s="16"/>
       <c r="AI22" s="6"/>
       <c r="AJ22" s="6"/>
       <c r="AK22" s="6"/>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23">
-        <v>23085163023</v>
+        <v>11538607113</v>
       </c>
       <c r="C23" s="8">
-        <f t="shared" si="18"/>
-        <v>10.363332945802444</v>
+        <f t="shared" si="13"/>
+        <v>10.062153385973239</v>
       </c>
       <c r="Z23" s="6"/>
       <c r="AA23" s="6"/>
@@ -4100,13 +5674,23 @@
       <c r="AD23" s="6"/>
       <c r="AE23" s="6"/>
       <c r="AF23" s="6"/>
-      <c r="AG23" s="16"/>
-      <c r="AH23" s="17"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
       <c r="AJ23" s="6"/>
       <c r="AK23" s="6"/>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>23085163023</v>
+      </c>
+      <c r="C24" s="8">
+        <f t="shared" si="13"/>
+        <v>10.363332945802444</v>
+      </c>
       <c r="Z24" s="6"/>
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
@@ -4114,14 +5698,28 @@
       <c r="AD24" s="6"/>
       <c r="AE24" s="6"/>
       <c r="AF24" s="6"/>
-      <c r="AG24" s="6"/>
-      <c r="AH24" s="6"/>
+      <c r="AG24" s="16"/>
+      <c r="AH24" s="17"/>
       <c r="AI24" s="6"/>
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="6"/>
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="6"/>
+      <c r="AG25" s="6"/>
+      <c r="AH25" s="6"/>
+      <c r="AI25" s="6"/>
+      <c r="AJ25" s="6"/>
+      <c r="AK25" s="6"/>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4137,6 +5735,20 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="W26" sqref="W26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
voortgang thesis + nieuwe metingen
</commit_message>
<xml_diff>
--- a/measurements/single-fold_single-iteration.xlsx
+++ b/measurements/single-fold_single-iteration.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="35">
   <si>
     <t>ListNet</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t xml:space="preserve">    - CUSTOM-50</t>
+  </si>
+  <si>
+    <t>Trainging2</t>
+  </si>
+  <si>
+    <t>Cluster (32 data nodes) (avanade)</t>
+  </si>
+  <si>
+    <t>Cluster (64 data nodes) (avanade)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - CUSTOM-100</t>
   </si>
 </sst>
 </file>
@@ -312,6 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -321,7 +334,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1141,7 +1153,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$BE$4:$BE$9</c:f>
+              <c:f>Sheet1!$BW$4:$BW$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1176,11 +1188,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="300498792"/>
-        <c:axId val="300499576"/>
+        <c:axId val="257226352"/>
+        <c:axId val="257231448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="300498792"/>
+        <c:axId val="257226352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1274,12 +1286,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300499576"/>
+        <c:crossAx val="257231448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="300499576"/>
+        <c:axId val="257231448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1374,7 +1386,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300498792"/>
+        <c:crossAx val="257226352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1847,8 +1859,264 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>24 data nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>143380</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4550507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5927007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25820919</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>838011150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2624103185</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5248206370</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13120515925</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26241031850</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52482063700</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>131205159250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AX$4:$AX$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="7">
+                  <c:v>485835</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>663075</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1046986</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2163385</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>32 data nodes</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>143380</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4550507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5927007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25820919</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>838011150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2624103185</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5248206370</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13120515925</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26241031850</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52482063700</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>131205159250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$BG$4:$BG$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="8">
+                  <c:v>681133</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>947447</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:v>ranklib</c:v>
           </c:tx>
@@ -1953,7 +2221,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$BE$4:$BE$12</c:f>
+              <c:f>Sheet1!$BW$4:$BW$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1988,11 +2256,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="250178896"/>
-        <c:axId val="250183992"/>
+        <c:axId val="257231840"/>
+        <c:axId val="257228704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="250178896"/>
+        <c:axId val="257231840"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2106,15 +2374,15 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="250183992"/>
+        <c:crossAx val="257228704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="250183992"/>
+        <c:axId val="257228704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2000000"/>
+          <c:max val="2200000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2226,7 +2494,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="250178896"/>
+        <c:crossAx val="257231840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -3765,10 +4033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BI27"/>
+  <dimension ref="A1:CA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT14" sqref="AT14"/>
+    <sheetView tabSelected="1" topLeftCell="AX1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BI17" sqref="BI17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3808,91 +4076,116 @@
     <col min="45" max="45" width="9.140625" style="6"/>
     <col min="48" max="48" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="49" max="52" width="10.7109375" customWidth="1"/>
-    <col min="55" max="55" width="9.140625" style="6"/>
-    <col min="56" max="56" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="63" width="9.140625" style="6"/>
+    <col min="64" max="64" width="14.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="65" max="73" width="9.140625" style="6"/>
+    <col min="74" max="74" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="23" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="23" t="s">
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="23" t="s">
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="23" t="s">
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
-      <c r="AO1" s="24"/>
-      <c r="AP1" s="24"/>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="25"/>
-      <c r="AT1" s="23" t="s">
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="AU1" s="24"/>
-      <c r="AV1" s="24"/>
-      <c r="AW1" s="24"/>
-      <c r="AX1" s="24"/>
-      <c r="AY1" s="24"/>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="24"/>
-      <c r="BB1" s="25"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="24" t="s">
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="25"/>
+      <c r="BB1" s="26"/>
+      <c r="BC1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="BD1" s="25"/>
+      <c r="BE1" s="25"/>
+      <c r="BF1" s="25"/>
+      <c r="BG1" s="25"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="26"/>
+      <c r="BL1" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="26"/>
+      <c r="BU1" s="13"/>
+      <c r="BV1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="BE1" s="24"/>
-      <c r="BF1" s="24"/>
-      <c r="BG1" s="24"/>
-      <c r="BH1" s="24"/>
-      <c r="BI1" s="24"/>
+      <c r="BW1" s="25"/>
+      <c r="BX1" s="25"/>
+      <c r="BY1" s="25"/>
+      <c r="BZ1" s="25"/>
+      <c r="CA1" s="25"/>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
       <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
@@ -4046,27 +4339,81 @@
       <c r="BB2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BC2" s="9"/>
-      <c r="BD2" s="2" t="s">
+      <c r="BC2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="BE2" s="3" t="s">
+      <c r="BD2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="BF2" s="3" t="s">
+      <c r="BE2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="BG2" s="3" t="s">
+      <c r="BF2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BG2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="BH2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="BI2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BJ2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BK2" s="12" t="s">
         <v>12</v>
       </c>
+      <c r="BL2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="BN2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="BO2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BP2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="BQ2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="BR2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BS2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="BT2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="BU2" s="9"/>
+      <c r="BV2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="BW2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="BX2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BY2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>11</v>
+      </c>
+      <c r="CA2" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4108,8 +4455,13 @@
       <c r="AJ3" s="8"/>
       <c r="AS3" s="8"/>
       <c r="BB3" s="8"/>
+      <c r="BC3" s="6"/>
+      <c r="BD3" s="6"/>
+      <c r="BE3" s="6"/>
+      <c r="BK3" s="8"/>
+      <c r="BT3" s="8"/>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>17</v>
       </c>
@@ -4245,29 +4597,34 @@
       <c r="AZ4" s="18"/>
       <c r="BA4" s="18"/>
       <c r="BB4" s="17"/>
-      <c r="BD4">
+      <c r="BC4" s="15"/>
+      <c r="BD4" s="15"/>
+      <c r="BE4" s="15"/>
+      <c r="BK4" s="8"/>
+      <c r="BT4" s="8"/>
+      <c r="BV4">
         <v>71</v>
       </c>
-      <c r="BE4">
+      <c r="BW4">
         <v>37</v>
       </c>
-      <c r="BF4">
-        <f>B4/BE4</f>
+      <c r="BX4">
+        <f t="shared" ref="BX4:BX9" si="6">B4/BW4</f>
         <v>3875.135135135135</v>
       </c>
-      <c r="BG4">
-        <f>LOG(BF4)</f>
+      <c r="BY4">
+        <f>LOG(BX4)</f>
         <v>3.5882868519830224</v>
       </c>
-      <c r="BH4">
+      <c r="BZ4">
         <v>4</v>
       </c>
-      <c r="BI4">
-        <f>SUM(BD4:BH4)</f>
+      <c r="CA4">
+        <f>SUM(BV4:BZ4)</f>
         <v>3990.7234219871179</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>3</v>
       </c>
@@ -4289,7 +4646,7 @@
         <v>13.617463723228207</v>
       </c>
       <c r="G5" s="15">
-        <f t="shared" ref="G5:G8" si="6">LOG(F5)</f>
+        <f t="shared" ref="G5:G8" si="7">LOG(F5)</f>
         <v>1.1340962269910448</v>
       </c>
       <c r="H5" s="16">
@@ -4340,7 +4697,7 @@
         <v>10.928945750434707</v>
       </c>
       <c r="V5" s="15">
-        <f t="shared" ref="V5:V8" si="7">LOG(U5)</f>
+        <f t="shared" ref="V5:V8" si="8">LOG(U5)</f>
         <v>1.0385782701975261</v>
       </c>
       <c r="W5" s="15">
@@ -4412,29 +4769,34 @@
       <c r="AZ5" s="18"/>
       <c r="BA5" s="18"/>
       <c r="BB5" s="17"/>
-      <c r="BD5">
+      <c r="BC5" s="15"/>
+      <c r="BD5" s="15"/>
+      <c r="BE5" s="15"/>
+      <c r="BK5" s="8"/>
+      <c r="BT5" s="8"/>
+      <c r="BV5">
         <v>236</v>
       </c>
-      <c r="BE5">
+      <c r="BW5">
         <v>109</v>
       </c>
-      <c r="BF5">
-        <f>B5/BE5</f>
+      <c r="BX5">
+        <f t="shared" si="6"/>
         <v>41747.770642201838</v>
       </c>
-      <c r="BG5">
-        <f t="shared" ref="BG5:BG9" si="8">LOG(BF5)</f>
+      <c r="BY5">
+        <f t="shared" ref="BY5:BY9" si="9">LOG(BX5)</f>
         <v>4.6206332888342159</v>
       </c>
-      <c r="BH5">
+      <c r="BZ5">
         <v>4</v>
       </c>
-      <c r="BI5">
-        <f t="shared" ref="BI5:BI8" si="9">SUM(BD5:BH5)</f>
+      <c r="CA5">
+        <f t="shared" ref="CA5:CA8" si="10">SUM(BV5:BZ5)</f>
         <v>42101.391275490671</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>15</v>
       </c>
@@ -4456,7 +4818,7 @@
         <v>17.928735854706929</v>
       </c>
       <c r="G6" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.2535496687769128</v>
       </c>
       <c r="H6" s="15">
@@ -4485,7 +4847,7 @@
         <v>12.916724599717126</v>
       </c>
       <c r="V6" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.1111523999895863</v>
       </c>
       <c r="W6" s="15">
@@ -4557,29 +4919,34 @@
       <c r="AZ6" s="18"/>
       <c r="BA6" s="18"/>
       <c r="BB6" s="17"/>
-      <c r="BD6">
+      <c r="BC6" s="15"/>
+      <c r="BD6" s="15"/>
+      <c r="BE6" s="15"/>
+      <c r="BK6" s="8"/>
+      <c r="BT6" s="8"/>
+      <c r="BV6">
         <v>229</v>
       </c>
-      <c r="BE6">
+      <c r="BW6">
         <v>142</v>
       </c>
-      <c r="BF6">
-        <f>B6/BE6</f>
+      <c r="BX6">
+        <f t="shared" si="6"/>
         <v>41739.485915492958</v>
       </c>
-      <c r="BG6">
-        <f t="shared" si="8"/>
+      <c r="BY6">
+        <f t="shared" si="9"/>
         <v>4.6205470957730492</v>
       </c>
-      <c r="BH6">
+      <c r="BZ6">
         <v>4</v>
       </c>
-      <c r="BI6">
-        <f t="shared" si="9"/>
+      <c r="CA6">
+        <f t="shared" si="10"/>
         <v>42119.10646258873</v>
       </c>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
@@ -4601,7 +4968,7 @@
         <v>81.560263055652953</v>
       </c>
       <c r="G7" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.9114786178348209</v>
       </c>
       <c r="H7" s="16">
@@ -4621,7 +4988,7 @@
         <v>73.581061672527483</v>
       </c>
       <c r="M7" s="16">
-        <f t="shared" ref="M7:M9" si="10">LOG(L7)</f>
+        <f t="shared" ref="M7:M9" si="11">LOG(L7)</f>
         <v>1.8667660498065228</v>
       </c>
       <c r="N7" s="15">
@@ -4632,7 +4999,7 @@
         <v>130.94768364733625</v>
       </c>
       <c r="P7" s="16">
-        <f t="shared" ref="P7:P9" si="11">LOG(O7)</f>
+        <f t="shared" ref="P7:P9" si="12">LOG(O7)</f>
         <v>2.1170978205308009</v>
       </c>
       <c r="Q7" s="15">
@@ -4652,7 +5019,7 @@
         <v>65.60859589389166</v>
       </c>
       <c r="V7" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.8169607434110107</v>
       </c>
       <c r="W7" s="15">
@@ -4737,29 +5104,34 @@
       <c r="AZ7" s="16"/>
       <c r="BA7" s="16"/>
       <c r="BB7" s="17"/>
-      <c r="BD7">
+      <c r="BC7" s="15"/>
+      <c r="BD7" s="15"/>
+      <c r="BE7" s="15"/>
+      <c r="BK7" s="8"/>
+      <c r="BT7" s="8"/>
+      <c r="BV7">
         <v>757</v>
       </c>
-      <c r="BE7">
+      <c r="BW7">
         <v>211</v>
       </c>
-      <c r="BF7">
-        <f>B7/BE7</f>
+      <c r="BX7">
+        <f t="shared" si="6"/>
         <v>122374.02369668246</v>
       </c>
-      <c r="BG7">
-        <f t="shared" si="8"/>
+      <c r="BY7">
+        <f t="shared" si="9"/>
         <v>5.0876892400117271</v>
       </c>
-      <c r="BH7">
+      <c r="BZ7">
         <v>7</v>
       </c>
-      <c r="BI7">
-        <f t="shared" si="9"/>
+      <c r="CA7">
+        <f t="shared" si="10"/>
         <v>123354.11138592247</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>4</v>
       </c>
@@ -4781,7 +5153,7 @@
         <v>935.62907378420084</v>
       </c>
       <c r="G8" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.9711037086350469</v>
       </c>
       <c r="H8" s="16">
@@ -4810,7 +5182,7 @@
         <v>1409.3316526968665</v>
       </c>
       <c r="V8" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.1490132060172549</v>
       </c>
       <c r="W8" s="15">
@@ -4842,7 +5214,7 @@
         <v>1312.2075170639512</v>
       </c>
       <c r="AE8" s="15">
-        <f t="shared" ref="AE8:AE13" si="12">LOG(AD8)</f>
+        <f t="shared" ref="AE8:AE13" si="13">LOG(AD8)</f>
         <v>3.1180025213118792</v>
       </c>
       <c r="AF8" s="15">
@@ -4874,7 +5246,7 @@
         <v>1175.8935900620072</v>
       </c>
       <c r="AN8" s="16">
-        <f t="shared" ref="AN8:AN9" si="13">LOG(AM8)</f>
+        <f t="shared" ref="AN8:AN9" si="14">LOG(AM8)</f>
         <v>3.0703680229817771</v>
       </c>
       <c r="AO8" s="16"/>
@@ -4909,29 +5281,34 @@
       <c r="BB8" s="17">
         <v>1544713</v>
       </c>
-      <c r="BD8" s="16">
+      <c r="BC8" s="15"/>
+      <c r="BD8" s="15"/>
+      <c r="BE8" s="15"/>
+      <c r="BK8" s="8"/>
+      <c r="BT8" s="8"/>
+      <c r="BV8" s="16">
         <v>27942</v>
       </c>
-      <c r="BE8" s="16">
+      <c r="BW8" s="16">
         <v>4526</v>
       </c>
-      <c r="BF8">
-        <f>B8/BE8</f>
+      <c r="BX8">
+        <f t="shared" si="6"/>
         <v>185154.916040654</v>
       </c>
-      <c r="BG8">
-        <f t="shared" si="8"/>
+      <c r="BY8">
+        <f t="shared" si="9"/>
         <v>5.2675352474736892</v>
       </c>
-      <c r="BH8" s="16">
+      <c r="BZ8" s="16">
         <v>255</v>
       </c>
-      <c r="BI8">
-        <f t="shared" si="9"/>
+      <c r="CA8">
+        <f t="shared" si="10"/>
         <v>217883.18357590146</v>
       </c>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>5</v>
       </c>
@@ -4959,7 +5336,7 @@
         <v>1430.5684677818556</v>
       </c>
       <c r="M9" s="16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.1555086482078778</v>
       </c>
       <c r="N9" s="15">
@@ -4970,7 +5347,7 @@
         <v>3555.4833925890598</v>
       </c>
       <c r="P9" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3.5508986544222787</v>
       </c>
       <c r="Q9" s="15">
@@ -4986,7 +5363,7 @@
         <v>908608</v>
       </c>
       <c r="U9" s="15">
-        <f>B22/T9</f>
+        <f>B23/T9</f>
         <v>2888.047634403395</v>
       </c>
       <c r="V9" s="15">
@@ -4997,7 +5374,7 @@
         <v>480568</v>
       </c>
       <c r="X9" s="15">
-        <f>B22/W9</f>
+        <f>B23/W9</f>
         <v>5460.4201382530673</v>
       </c>
       <c r="Y9" s="15">
@@ -5022,7 +5399,7 @@
         <v>2870.9001132341759</v>
       </c>
       <c r="AE9" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.4580180824213178</v>
       </c>
       <c r="AF9" s="15">
@@ -5054,7 +5431,7 @@
         <v>3116.0050977453789</v>
       </c>
       <c r="AN9" s="16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.4935981595014503</v>
       </c>
       <c r="AO9" s="16"/>
@@ -5089,29 +5466,34 @@
       <c r="BB9" s="17">
         <v>1460980</v>
       </c>
-      <c r="BD9" s="16">
+      <c r="BC9" s="15"/>
+      <c r="BD9" s="15"/>
+      <c r="BE9" s="15"/>
+      <c r="BK9" s="8"/>
+      <c r="BT9" s="8"/>
+      <c r="BV9" s="16">
         <v>92778</v>
       </c>
-      <c r="BE9" s="16">
+      <c r="BW9" s="16">
         <v>14309</v>
       </c>
-      <c r="BF9">
-        <f>B9/BE9</f>
+      <c r="BX9">
+        <f t="shared" si="6"/>
         <v>183388.30002096583</v>
       </c>
-      <c r="BG9">
-        <f t="shared" si="8"/>
+      <c r="BY9">
+        <f t="shared" si="9"/>
         <v>5.2633716246905005</v>
       </c>
-      <c r="BH9" s="16">
+      <c r="BZ9" s="16">
         <v>107873</v>
       </c>
-      <c r="BI9">
-        <f>SUM(BD9:BH9)</f>
+      <c r="CA9">
+        <f>SUM(BV9:BZ9)</f>
         <v>398353.56339259056</v>
       </c>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>6</v>
       </c>
@@ -5145,7 +5527,7 @@
         <v>1514885</v>
       </c>
       <c r="U10" s="15">
-        <f>B23/T10</f>
+        <f>B24/T10</f>
         <v>3045.3154074401687</v>
       </c>
       <c r="V10" s="15">
@@ -5156,7 +5538,7 @@
         <v>751593</v>
       </c>
       <c r="X10" s="15">
-        <f>B23/W10</f>
+        <f>B24/W10</f>
         <v>6138.0329925904043</v>
       </c>
       <c r="Y10" s="15">
@@ -5181,7 +5563,7 @@
         <v>4873.1719313362901</v>
       </c>
       <c r="AE10" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.687811734080535</v>
       </c>
       <c r="AF10" s="15">
@@ -5213,18 +5595,29 @@
       <c r="AS10" s="17"/>
       <c r="AT10" s="18"/>
       <c r="AU10" s="18"/>
-      <c r="AV10" s="18"/>
-      <c r="AW10" s="18"/>
+      <c r="AV10" s="16" t="e">
+        <f t="shared" ref="AV10:AV14" si="15">B10/AU10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AW10" s="16" t="e">
+        <f t="shared" ref="AW10:AW14" si="16">LOG(AV10)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="AX10" s="18"/>
       <c r="AY10" s="18"/>
       <c r="AZ10" s="18"/>
       <c r="BA10" s="18"/>
       <c r="BB10" s="17"/>
-      <c r="BD10" t="s">
+      <c r="BC10" s="15"/>
+      <c r="BD10" s="15"/>
+      <c r="BE10" s="15"/>
+      <c r="BK10" s="8"/>
+      <c r="BT10" s="8"/>
+      <c r="BV10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>7</v>
       </c>
@@ -5258,7 +5651,7 @@
         <v>1879565</v>
       </c>
       <c r="U11" s="15">
-        <f>B24/T11</f>
+        <f>B25/T11</f>
         <v>6138.9774298840421</v>
       </c>
       <c r="V11" s="15">
@@ -5269,7 +5662,7 @@
         <v>1037886</v>
       </c>
       <c r="X11" s="15">
-        <f>B24/W11</f>
+        <f>B25/W11</f>
         <v>11117.412811233604</v>
       </c>
       <c r="Y11" s="15">
@@ -5301,7 +5694,7 @@
         <v>789234</v>
       </c>
       <c r="AG11" s="15">
-        <f>B24/AF11</f>
+        <f>B25/AF11</f>
         <v>14620.007644120755</v>
       </c>
       <c r="AH11" s="15">
@@ -5324,20 +5717,48 @@
       <c r="AQ11" s="18"/>
       <c r="AR11" s="18"/>
       <c r="AS11" s="17"/>
-      <c r="AT11" s="18"/>
-      <c r="AU11" s="18"/>
-      <c r="AV11" s="18"/>
-      <c r="AW11" s="18"/>
-      <c r="AX11" s="18"/>
-      <c r="AY11" s="18"/>
-      <c r="AZ11" s="18"/>
-      <c r="BA11" s="18"/>
-      <c r="BB11" s="17"/>
-      <c r="BD11" t="s">
+      <c r="AT11" s="18">
+        <v>969436</v>
+      </c>
+      <c r="AU11" s="18">
+        <v>1187552</v>
+      </c>
+      <c r="AV11" s="16">
+        <f t="shared" si="15"/>
+        <v>11048.371713407076</v>
+      </c>
+      <c r="AW11" s="16">
+        <f t="shared" si="16"/>
+        <v>4.0432982772981152</v>
+      </c>
+      <c r="AX11" s="18">
+        <v>485835</v>
+      </c>
+      <c r="AY11">
+        <f>B11/AX11</f>
+        <v>27006.115090514268</v>
+      </c>
+      <c r="AZ11">
+        <f>LOG(AY11)</f>
+        <v>4.4314621141355994</v>
+      </c>
+      <c r="BA11" s="18">
+        <v>243331</v>
+      </c>
+      <c r="BB11" s="8">
+        <f>SUM(BA11,AX11,AU11,AT11)</f>
+        <v>2886154</v>
+      </c>
+      <c r="BC11" s="15"/>
+      <c r="BD11" s="15"/>
+      <c r="BE11" s="15"/>
+      <c r="BK11" s="8"/>
+      <c r="BT11" s="8"/>
+      <c r="BV11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>8</v>
       </c>
@@ -5371,7 +5792,7 @@
         <v>3304425</v>
       </c>
       <c r="U12" s="15">
-        <f>B25/T12</f>
+        <f>B26/T12</f>
         <v>6986.136172859121</v>
       </c>
       <c r="V12" s="15">
@@ -5382,7 +5803,7 @@
         <v>1715801</v>
       </c>
       <c r="X12" s="15">
-        <f>B25/W12</f>
+        <f>B26/W12</f>
         <v>13454.452481960321</v>
       </c>
       <c r="Y12" s="15">
@@ -5393,7 +5814,7 @@
         <v>287681</v>
       </c>
       <c r="AA12" s="17">
-        <f t="shared" ref="AA12" si="14">SUM(S12:T12,W12,Z12)</f>
+        <f t="shared" ref="AA12" si="17">SUM(S12:T12,W12,Z12)</f>
         <v>7230333</v>
       </c>
       <c r="AB12" s="15">
@@ -5407,7 +5828,7 @@
         <v>12879.988578294637</v>
       </c>
       <c r="AE12" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.109915477900671</v>
       </c>
       <c r="AF12" s="15">
@@ -5425,7 +5846,7 @@
         <v>201019</v>
       </c>
       <c r="AJ12" s="8">
-        <f t="shared" ref="AJ12:AJ13" si="15">SUM(AI12,AF12,AC12,AB12)</f>
+        <f t="shared" ref="AJ12:AJ13" si="18">SUM(AI12,AF12,AC12,AB12)</f>
         <v>4234435</v>
       </c>
       <c r="AK12" s="18"/>
@@ -5437,20 +5858,76 @@
       <c r="AQ12" s="18"/>
       <c r="AR12" s="18"/>
       <c r="AS12" s="17"/>
-      <c r="AT12" s="18"/>
-      <c r="AU12" s="18"/>
-      <c r="AV12" s="18"/>
-      <c r="AW12" s="18"/>
-      <c r="AX12" s="18"/>
-      <c r="AY12" s="18"/>
-      <c r="AZ12" s="18"/>
-      <c r="BA12" s="18"/>
-      <c r="BB12" s="17"/>
-      <c r="BD12" t="s">
+      <c r="AT12" s="18">
+        <v>997748</v>
+      </c>
+      <c r="AU12" s="18">
+        <v>1426485</v>
+      </c>
+      <c r="AV12" s="16">
+        <f t="shared" si="15"/>
+        <v>18395.589052811632</v>
+      </c>
+      <c r="AW12" s="16">
+        <f t="shared" si="16"/>
+        <v>4.2647136991141261</v>
+      </c>
+      <c r="AX12" s="18">
+        <v>663075</v>
+      </c>
+      <c r="AY12">
+        <f>B12/AX12</f>
+        <v>39574.756777136827</v>
+      </c>
+      <c r="AZ12">
+        <f>LOG(AY12)</f>
+        <v>4.5974182544081286</v>
+      </c>
+      <c r="BA12" s="18">
+        <v>243764</v>
+      </c>
+      <c r="BB12" s="8">
+        <f>SUM(BA12,AX12,AU12,AT12)</f>
+        <v>3331072</v>
+      </c>
+      <c r="BC12" s="6">
+        <v>1295244</v>
+      </c>
+      <c r="BD12" s="6">
+        <v>1257854</v>
+      </c>
+      <c r="BE12" s="16">
+        <f>B12/BD12</f>
+        <v>20861.746951553996</v>
+      </c>
+      <c r="BF12" s="6">
+        <f>LOG(BE12)</f>
+        <v>4.3193506732013924</v>
+      </c>
+      <c r="BG12" s="6">
+        <v>681133</v>
+      </c>
+      <c r="BH12">
+        <f>B12/BG12</f>
+        <v>38525.562335109295</v>
+      </c>
+      <c r="BI12">
+        <f>LOG(BH12)</f>
+        <v>4.5857489865793619</v>
+      </c>
+      <c r="BJ12" s="6">
+        <v>419077</v>
+      </c>
+      <c r="BK12" s="8">
+        <f>SUM(BJ12,BG12,BD12,BC12)</f>
+        <v>3653308</v>
+      </c>
+      <c r="BT12" s="8"/>
+      <c r="BV12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>29</v>
       </c>
@@ -5480,7 +5957,7 @@
         <v>14188.329611566494</v>
       </c>
       <c r="AE13" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.1519312690881582</v>
       </c>
       <c r="AF13" s="15">
@@ -5498,14 +5975,80 @@
         <v>199887</v>
       </c>
       <c r="AJ13" s="8">
+        <f t="shared" si="18"/>
+        <v>8174345</v>
+      </c>
+      <c r="AS13" s="8"/>
+      <c r="AT13">
+        <v>1496779</v>
+      </c>
+      <c r="AU13">
+        <v>1714057</v>
+      </c>
+      <c r="AV13" s="16">
         <f t="shared" si="15"/>
-        <v>8174345</v>
-      </c>
-      <c r="AS13" s="8"/>
-      <c r="BB13" s="8"/>
+        <v>30618.622192844228</v>
+      </c>
+      <c r="AW13" s="16">
+        <f t="shared" si="16"/>
+        <v>4.4859856439877221</v>
+      </c>
+      <c r="AX13">
+        <v>1046986</v>
+      </c>
+      <c r="AY13">
+        <f>B13/AX13</f>
+        <v>50126.805611536351</v>
+      </c>
+      <c r="AZ13">
+        <f>LOG(AY13)</f>
+        <v>4.7000700295784297</v>
+      </c>
+      <c r="BA13">
+        <v>391366</v>
+      </c>
+      <c r="BB13" s="8">
+        <f>SUM(BA13,AX13,AU13,AT13)</f>
+        <v>4649188</v>
+      </c>
+      <c r="BC13" s="6">
+        <v>1338189</v>
+      </c>
+      <c r="BD13" s="6">
+        <v>2078534</v>
+      </c>
+      <c r="BE13" s="16">
+        <f>B13/BD13</f>
+        <v>25249.557476567621</v>
+      </c>
+      <c r="BF13" s="6">
+        <f>LOG(BE13)</f>
+        <v>4.4022537710816545</v>
+      </c>
+      <c r="BG13" s="6">
+        <v>947447</v>
+      </c>
+      <c r="BH13">
+        <f>B13/BG13</f>
+        <v>55393.139352385937</v>
+      </c>
+      <c r="BI13">
+        <f>LOG(BH13)</f>
+        <v>4.7434559790622357</v>
+      </c>
+      <c r="BJ13" s="6">
+        <v>421768</v>
+      </c>
+      <c r="BK13" s="8">
+        <v>4785939</v>
+      </c>
+      <c r="BT13" s="8"/>
+      <c r="BV13" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="21">
@@ -5533,56 +6076,100 @@
       <c r="AI14" s="16"/>
       <c r="AJ14" s="8"/>
       <c r="AS14" s="8"/>
-      <c r="BB14" s="8"/>
+      <c r="AT14">
+        <v>2136358</v>
+      </c>
+      <c r="AU14">
+        <v>3832440</v>
+      </c>
+      <c r="AV14" s="16">
+        <f t="shared" si="15"/>
+        <v>34235.411187128826</v>
+      </c>
+      <c r="AW14" s="16">
+        <f t="shared" si="16"/>
+        <v>4.5344755483630772</v>
+      </c>
+      <c r="AX14">
+        <v>2163385</v>
+      </c>
+      <c r="AY14">
+        <f>B14/AX14</f>
+        <v>60648.085870060117</v>
+      </c>
+      <c r="AZ14">
+        <f>LOG(AY14)</f>
+        <v>4.7828170985383087</v>
+      </c>
+      <c r="BA14">
+        <v>379087</v>
+      </c>
+      <c r="BB14" s="8">
+        <f>SUM(BA14,AX14,AU14,AT14)</f>
+        <v>8511270</v>
+      </c>
+      <c r="BC14" s="6"/>
+      <c r="BD14" s="6"/>
+      <c r="BE14" s="6"/>
+      <c r="BK14" s="8"/>
+      <c r="BT14" s="8"/>
+      <c r="BV14" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="21">
+        <f>100*B9</f>
+        <v>262410318500</v>
+      </c>
+      <c r="C15" s="22">
+        <f>LOG(B15)</f>
+        <v>11.418980908369416</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="R15" s="8"/>
       <c r="U15" s="15"/>
       <c r="V15" s="15"/>
       <c r="X15" s="15"/>
       <c r="Y15" s="15"/>
-      <c r="AA15" s="15"/>
+      <c r="AA15" s="17"/>
       <c r="AD15" s="15"/>
       <c r="AE15" s="15"/>
       <c r="AF15" s="15"/>
       <c r="AG15" s="15"/>
       <c r="AH15" s="15"/>
+      <c r="AJ15" s="8"/>
+      <c r="AS15" s="8"/>
+      <c r="BB15" s="8"/>
+      <c r="BK15" s="8"/>
+      <c r="BT15" s="8"/>
+      <c r="BV15" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="8"/>
+    <row r="16" spans="1:79" x14ac:dyDescent="0.25">
       <c r="U16" s="15"/>
       <c r="V16" s="15"/>
       <c r="X16" s="15"/>
       <c r="Y16" s="15"/>
-      <c r="Z16" s="6"/>
       <c r="AA16" s="15"/>
-      <c r="AB16" s="6"/>
-      <c r="AC16" s="6"/>
       <c r="AD16" s="15"/>
       <c r="AE16" s="15"/>
       <c r="AF16" s="15"/>
       <c r="AG16" s="15"/>
       <c r="AH16" s="15"/>
-      <c r="AI16" s="6"/>
-      <c r="AJ16" s="6"/>
-      <c r="AK16" s="6"/>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>143380</v>
-      </c>
-      <c r="C17" s="8">
-        <f t="shared" ref="C17:C25" si="16">LOG(B17)</f>
-        <v>5.156488576050017</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8"/>
       <c r="U17" s="15"/>
       <c r="V17" s="15"/>
       <c r="X17" s="15"/>
@@ -5602,14 +6189,14 @@
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>4550507</v>
+        <v>143380</v>
       </c>
       <c r="C18" s="8">
-        <f t="shared" si="16"/>
-        <v>6.6580597867748397</v>
+        <f t="shared" ref="C18:C26" si="19">LOG(B18)</f>
+        <v>5.156488576050017</v>
       </c>
       <c r="U18" s="15"/>
       <c r="V18" s="15"/>
@@ -5630,14 +6217,14 @@
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B19">
-        <v>5927007</v>
+        <v>4550507</v>
       </c>
       <c r="C19" s="8">
-        <f t="shared" si="16"/>
-        <v>6.7728354401561059</v>
+        <f t="shared" si="19"/>
+        <v>6.6580597867748397</v>
       </c>
       <c r="U19" s="15"/>
       <c r="V19" s="15"/>
@@ -5658,14 +6245,14 @@
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20">
-        <v>25820919</v>
+        <v>5927007</v>
       </c>
       <c r="C20" s="8">
-        <f t="shared" si="16"/>
-        <v>7.4119716953094192</v>
+        <f t="shared" si="19"/>
+        <v>6.7728354401561059</v>
       </c>
       <c r="U20" s="15"/>
       <c r="V20" s="15"/>
@@ -5686,14 +6273,14 @@
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B21">
-        <v>838011150</v>
+        <v>25820919</v>
       </c>
       <c r="C21" s="8">
-        <f t="shared" si="16"/>
-        <v>8.9232497970923994</v>
+        <f t="shared" si="19"/>
+        <v>7.4119716953094192</v>
       </c>
       <c r="U21" s="15"/>
       <c r="V21" s="15"/>
@@ -5714,22 +6301,26 @@
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22">
-        <v>2624103185</v>
+        <v>838011150</v>
       </c>
       <c r="C22" s="8">
-        <f t="shared" si="16"/>
-        <v>9.4189809083694165</v>
-      </c>
+        <f t="shared" si="19"/>
+        <v>8.9232497970923994</v>
+      </c>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
       <c r="Z22" s="6"/>
-      <c r="AA22" s="6"/>
+      <c r="AA22" s="15"/>
       <c r="AB22" s="6"/>
       <c r="AC22" s="6"/>
       <c r="AD22" s="15"/>
       <c r="AE22" s="15"/>
-      <c r="AF22" s="6"/>
+      <c r="AF22" s="15"/>
       <c r="AG22" s="15"/>
       <c r="AH22" s="15"/>
       <c r="AI22" s="6"/>
@@ -5738,14 +6329,14 @@
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23">
-        <v>4613302631</v>
+        <v>2624103185</v>
       </c>
       <c r="C23" s="8">
-        <f t="shared" si="16"/>
-        <v>9.664011945105198</v>
+        <f t="shared" si="19"/>
+        <v>9.4189809083694165</v>
       </c>
       <c r="Z23" s="6"/>
       <c r="AA23" s="6"/>
@@ -5762,38 +6353,38 @@
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24">
-        <v>11538607113</v>
+        <v>4613302631</v>
       </c>
       <c r="C24" s="8">
-        <f t="shared" si="16"/>
-        <v>10.062153385973239</v>
+        <f t="shared" si="19"/>
+        <v>9.664011945105198</v>
       </c>
       <c r="Z24" s="6"/>
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
       <c r="AC24" s="6"/>
-      <c r="AD24" s="6"/>
-      <c r="AE24" s="6"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="15"/>
       <c r="AF24" s="6"/>
-      <c r="AG24" s="6"/>
-      <c r="AH24" s="6"/>
+      <c r="AG24" s="15"/>
+      <c r="AH24" s="15"/>
       <c r="AI24" s="6"/>
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25">
-        <v>23085163023</v>
+        <v>11538607113</v>
       </c>
       <c r="C25" s="8">
-        <f t="shared" si="16"/>
-        <v>10.363332945802444</v>
+        <f t="shared" si="19"/>
+        <v>10.062153385973239</v>
       </c>
       <c r="Z25" s="6"/>
       <c r="AA25" s="6"/>
@@ -5802,13 +6393,23 @@
       <c r="AD25" s="6"/>
       <c r="AE25" s="6"/>
       <c r="AF25" s="6"/>
-      <c r="AG25" s="15"/>
-      <c r="AH25" s="16"/>
+      <c r="AG25" s="6"/>
+      <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
       <c r="AJ25" s="6"/>
       <c r="AK25" s="6"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>23085163023</v>
+      </c>
+      <c r="C26" s="8">
+        <f t="shared" si="19"/>
+        <v>10.363332945802444</v>
+      </c>
       <c r="Z26" s="6"/>
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
@@ -5816,26 +6417,42 @@
       <c r="AD26" s="6"/>
       <c r="AE26" s="6"/>
       <c r="AF26" s="6"/>
-      <c r="AG26" s="6"/>
-      <c r="AH26" s="6"/>
+      <c r="AG26" s="15"/>
+      <c r="AH26" s="16"/>
       <c r="AI26" s="6"/>
       <c r="AJ26" s="6"/>
       <c r="AK26" s="6"/>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="6"/>
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="6"/>
+      <c r="AE27" s="6"/>
+      <c r="AF27" s="6"/>
+      <c r="AG27" s="6"/>
+      <c r="AH27" s="6"/>
+      <c r="AI27" s="6"/>
+      <c r="AJ27" s="6"/>
+      <c r="AK27" s="6"/>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="S1:AA1"/>
-    <mergeCell ref="BD1:BI1"/>
+    <mergeCell ref="BV1:CA1"/>
     <mergeCell ref="AK1:AS1"/>
     <mergeCell ref="AT1:BB1"/>
     <mergeCell ref="J1:R1"/>
     <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="BC1:BK1"/>
+    <mergeCell ref="BL1:BT1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5846,8 +6463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="W26" sqref="W26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
mooie plaatjes + in report
</commit_message>
<xml_diff>
--- a/measurements/single-fold_single-iteration.xlsx
+++ b/measurements/single-fold_single-iteration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12360"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -324,6 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -333,7 +334,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1188,11 +1188,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257226352"/>
-        <c:axId val="257231448"/>
+        <c:axId val="302212984"/>
+        <c:axId val="302213376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="257226352"/>
+        <c:axId val="302212984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,12 +1286,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257231448"/>
+        <c:crossAx val="302213376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="257231448"/>
+        <c:axId val="302213376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1386,7 +1386,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257226352"/>
+        <c:crossAx val="302212984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2259,11 +2259,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257231840"/>
-        <c:axId val="257228704"/>
+        <c:axId val="302214552"/>
+        <c:axId val="302212200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="257231840"/>
+        <c:axId val="302214552"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2377,12 +2377,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257228704"/>
+        <c:crossAx val="302212200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="257228704"/>
+        <c:axId val="302212200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200000"/>
@@ -2497,7 +2497,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257231840"/>
+        <c:crossAx val="302214552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -4038,8 +4038,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BK15" sqref="BK15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AZ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B12" sqref="B12:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4093,100 +4094,100 @@
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="23" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="23" t="s">
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="23" t="s">
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="23" t="s">
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
-      <c r="AO1" s="24"/>
-      <c r="AP1" s="24"/>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="25"/>
-      <c r="AT1" s="23" t="s">
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="AU1" s="24"/>
-      <c r="AV1" s="24"/>
-      <c r="AW1" s="24"/>
-      <c r="AX1" s="24"/>
-      <c r="AY1" s="24"/>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="24"/>
-      <c r="BB1" s="25"/>
-      <c r="BC1" s="23" t="s">
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="25"/>
+      <c r="BB1" s="26"/>
+      <c r="BC1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="BD1" s="24"/>
-      <c r="BE1" s="24"/>
-      <c r="BF1" s="24"/>
-      <c r="BG1" s="24"/>
-      <c r="BH1" s="24"/>
-      <c r="BI1" s="24"/>
-      <c r="BJ1" s="24"/>
-      <c r="BK1" s="25"/>
-      <c r="BL1" s="23" t="s">
+      <c r="BD1" s="25"/>
+      <c r="BE1" s="25"/>
+      <c r="BF1" s="25"/>
+      <c r="BG1" s="25"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="26"/>
+      <c r="BL1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="BM1" s="24"/>
-      <c r="BN1" s="24"/>
-      <c r="BO1" s="24"/>
-      <c r="BP1" s="24"/>
-      <c r="BQ1" s="24"/>
-      <c r="BR1" s="24"/>
-      <c r="BS1" s="24"/>
-      <c r="BT1" s="25"/>
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="26"/>
       <c r="BU1" s="13"/>
-      <c r="BV1" s="24" t="s">
+      <c r="BV1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="BW1" s="24"/>
-      <c r="BX1" s="24"/>
-      <c r="BY1" s="24"/>
-      <c r="BZ1" s="24"/>
-      <c r="CA1" s="24"/>
+      <c r="BW1" s="25"/>
+      <c r="BX1" s="25"/>
+      <c r="BY1" s="25"/>
+      <c r="BZ1" s="25"/>
+      <c r="CA1" s="25"/>
     </row>
     <row r="2" spans="1:79" x14ac:dyDescent="0.25">
       <c r="D2" s="10" t="s">
@@ -6051,7 +6052,7 @@
       </c>
     </row>
     <row r="14" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="23" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="21">
@@ -6494,7 +6495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
nieuwer serial meting + hernoeming scripts
</commit_message>
<xml_diff>
--- a/measurements/single-fold_single-iteration.xlsx
+++ b/measurements/single-fold_single-iteration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="35">
   <si>
     <t>ListNet</t>
   </si>
@@ -1170,7 +1170,7 @@
                   <c:v>211</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4526</c:v>
+                  <c:v>4566</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>14309</c:v>
@@ -1188,11 +1188,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="302212984"/>
-        <c:axId val="302213376"/>
+        <c:axId val="266206496"/>
+        <c:axId val="266212376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="302212984"/>
+        <c:axId val="266206496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,12 +1286,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302213376"/>
+        <c:crossAx val="266212376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="302213376"/>
+        <c:axId val="266212376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1386,7 +1386,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302212984"/>
+        <c:crossAx val="266206496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2224,27 +2224,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$BW$4:$BW$12</c:f>
+              <c:f>Sheet1!$BU$4:$BU$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>37</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>109</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>142</c:v>
+                  <c:v>371</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>211</c:v>
+                  <c:v>968</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4526</c:v>
+                  <c:v>32508</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14309</c:v>
+                  <c:v>107087</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>170968</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>480878</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2259,11 +2265,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="302214552"/>
-        <c:axId val="302212200"/>
+        <c:axId val="266210808"/>
+        <c:axId val="266205712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="302214552"/>
+        <c:axId val="266210808"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2377,12 +2383,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302212200"/>
+        <c:crossAx val="266205712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="302212200"/>
+        <c:axId val="266205712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200000"/>
@@ -2497,7 +2503,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302214552"/>
+        <c:crossAx val="266210808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -4038,9 +4044,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AZ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B12" sqref="B12:B14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BW10" sqref="BW10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4085,6 +4091,7 @@
     <col min="64" max="64" width="14.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="65" max="73" width="9.140625" style="6"/>
     <col min="74" max="74" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="7.42578125" customWidth="1"/>
     <col min="77" max="77" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4606,6 +4613,10 @@
       <c r="BE4" s="15"/>
       <c r="BK4" s="8"/>
       <c r="BT4" s="8"/>
+      <c r="BU4" s="6">
+        <f>BV4+BW4</f>
+        <v>108</v>
+      </c>
       <c r="BV4">
         <v>71</v>
       </c>
@@ -4613,7 +4624,7 @@
         <v>37</v>
       </c>
       <c r="BX4">
-        <f t="shared" ref="BX4:BX9" si="6">B4/BW4</f>
+        <f t="shared" ref="BX4:BX11" si="6">B4/BW4</f>
         <v>3875.135135135135</v>
       </c>
       <c r="BY4">
@@ -4778,6 +4789,10 @@
       <c r="BE5" s="15"/>
       <c r="BK5" s="8"/>
       <c r="BT5" s="8"/>
+      <c r="BU5" s="6">
+        <f t="shared" ref="BU5:BU11" si="9">BV5+BW5</f>
+        <v>345</v>
+      </c>
       <c r="BV5">
         <v>236</v>
       </c>
@@ -4789,14 +4804,14 @@
         <v>41747.770642201838</v>
       </c>
       <c r="BY5">
-        <f t="shared" ref="BY5:BY9" si="9">LOG(BX5)</f>
+        <f t="shared" ref="BY5:BY11" si="10">LOG(BX5)</f>
         <v>4.6206332888342159</v>
       </c>
       <c r="BZ5">
         <v>4</v>
       </c>
       <c r="CA5">
-        <f t="shared" ref="CA5:CA8" si="10">SUM(BV5:BZ5)</f>
+        <f t="shared" ref="CA5:CA8" si="11">SUM(BV5:BZ5)</f>
         <v>42101.391275490671</v>
       </c>
     </row>
@@ -4928,6 +4943,10 @@
       <c r="BE6" s="15"/>
       <c r="BK6" s="8"/>
       <c r="BT6" s="8"/>
+      <c r="BU6" s="6">
+        <f t="shared" si="9"/>
+        <v>371</v>
+      </c>
       <c r="BV6">
         <v>229</v>
       </c>
@@ -4939,14 +4958,14 @@
         <v>41739.485915492958</v>
       </c>
       <c r="BY6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.6205470957730492</v>
       </c>
       <c r="BZ6">
         <v>4</v>
       </c>
       <c r="CA6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>42119.10646258873</v>
       </c>
     </row>
@@ -4992,7 +5011,7 @@
         <v>73.581061672527483</v>
       </c>
       <c r="M7" s="16">
-        <f t="shared" ref="M7:M9" si="11">LOG(L7)</f>
+        <f t="shared" ref="M7:M9" si="12">LOG(L7)</f>
         <v>1.8667660498065228</v>
       </c>
       <c r="N7" s="15">
@@ -5003,7 +5022,7 @@
         <v>130.94768364733625</v>
       </c>
       <c r="P7" s="16">
-        <f t="shared" ref="P7:P9" si="12">LOG(O7)</f>
+        <f t="shared" ref="P7:P9" si="13">LOG(O7)</f>
         <v>2.1170978205308009</v>
       </c>
       <c r="Q7" s="15">
@@ -5113,6 +5132,10 @@
       <c r="BE7" s="15"/>
       <c r="BK7" s="8"/>
       <c r="BT7" s="8"/>
+      <c r="BU7" s="6">
+        <f t="shared" si="9"/>
+        <v>968</v>
+      </c>
       <c r="BV7">
         <v>757</v>
       </c>
@@ -5124,14 +5147,14 @@
         <v>122374.02369668246</v>
       </c>
       <c r="BY7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.0876892400117271</v>
       </c>
       <c r="BZ7">
         <v>7</v>
       </c>
       <c r="CA7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>123354.11138592247</v>
       </c>
     </row>
@@ -5218,7 +5241,7 @@
         <v>1312.2075170639512</v>
       </c>
       <c r="AE8" s="15">
-        <f t="shared" ref="AE8:AE13" si="13">LOG(AD8)</f>
+        <f t="shared" ref="AE8:AE13" si="14">LOG(AD8)</f>
         <v>3.1180025213118792</v>
       </c>
       <c r="AF8" s="15">
@@ -5250,7 +5273,7 @@
         <v>1175.8935900620072</v>
       </c>
       <c r="AN8" s="16">
-        <f t="shared" ref="AN8:AN9" si="14">LOG(AM8)</f>
+        <f t="shared" ref="AN8:AN9" si="15">LOG(AM8)</f>
         <v>3.0703680229817771</v>
       </c>
       <c r="AO8" s="16"/>
@@ -5290,26 +5313,30 @@
       <c r="BE8" s="15"/>
       <c r="BK8" s="8"/>
       <c r="BT8" s="8"/>
+      <c r="BU8" s="6">
+        <f t="shared" si="9"/>
+        <v>32508</v>
+      </c>
       <c r="BV8" s="16">
         <v>27942</v>
       </c>
       <c r="BW8" s="16">
-        <v>4526</v>
+        <v>4566</v>
       </c>
       <c r="BX8">
         <f t="shared" si="6"/>
-        <v>185154.916040654</v>
+        <v>183532.88436268069</v>
       </c>
       <c r="BY8">
-        <f t="shared" si="9"/>
-        <v>5.2675352474736892</v>
+        <f t="shared" si="10"/>
+        <v>5.2637138899381819</v>
       </c>
       <c r="BZ8" s="16">
         <v>255</v>
       </c>
       <c r="CA8">
-        <f t="shared" si="10"/>
-        <v>217883.18357590146</v>
+        <f t="shared" si="11"/>
+        <v>216301.14807657062</v>
       </c>
     </row>
     <row r="9" spans="1:79" x14ac:dyDescent="0.25">
@@ -5340,7 +5367,7 @@
         <v>1430.5684677818556</v>
       </c>
       <c r="M9" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3.1555086482078778</v>
       </c>
       <c r="N9" s="15">
@@ -5351,7 +5378,7 @@
         <v>3555.4833925890598</v>
       </c>
       <c r="P9" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.5508986544222787</v>
       </c>
       <c r="Q9" s="15">
@@ -5403,7 +5430,7 @@
         <v>2870.9001132341759</v>
       </c>
       <c r="AE9" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.4580180824213178</v>
       </c>
       <c r="AF9" s="15">
@@ -5435,7 +5462,7 @@
         <v>3116.0050977453789</v>
       </c>
       <c r="AN9" s="16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.4935981595014503</v>
       </c>
       <c r="AO9" s="16"/>
@@ -5475,6 +5502,10 @@
       <c r="BE9" s="15"/>
       <c r="BK9" s="8"/>
       <c r="BT9" s="8"/>
+      <c r="BU9" s="6">
+        <f t="shared" si="9"/>
+        <v>107087</v>
+      </c>
       <c r="BV9" s="16">
         <v>92778</v>
       </c>
@@ -5486,15 +5517,15 @@
         <v>183388.30002096583</v>
       </c>
       <c r="BY9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.2633716246905005</v>
       </c>
       <c r="BZ9" s="16">
-        <v>107873</v>
+        <v>1078</v>
       </c>
       <c r="CA9">
         <f>SUM(BV9:BZ9)</f>
-        <v>398353.56339259056</v>
+        <v>291558.56339259056</v>
       </c>
     </row>
     <row r="10" spans="1:79" x14ac:dyDescent="0.25">
@@ -5567,7 +5598,7 @@
         <v>4873.1719313362901</v>
       </c>
       <c r="AE10" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.687811734080535</v>
       </c>
       <c r="AF10" s="15">
@@ -5600,11 +5631,11 @@
       <c r="AT10" s="18"/>
       <c r="AU10" s="18"/>
       <c r="AV10" s="16" t="e">
-        <f t="shared" ref="AV10:AV14" si="15">B10/AU10</f>
+        <f t="shared" ref="AV10:AV14" si="16">B10/AU10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AW10" s="16" t="e">
-        <f t="shared" ref="AW10:AW14" si="16">LOG(AV10)</f>
+        <f t="shared" ref="AW10:AW14" si="17">LOG(AV10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AX10" s="18"/>
@@ -5617,8 +5648,30 @@
       <c r="BE10" s="15"/>
       <c r="BK10" s="8"/>
       <c r="BT10" s="8"/>
-      <c r="BV10" t="s">
-        <v>23</v>
+      <c r="BU10" s="6">
+        <f t="shared" si="9"/>
+        <v>170968</v>
+      </c>
+      <c r="BV10">
+        <v>142503</v>
+      </c>
+      <c r="BW10">
+        <v>28465</v>
+      </c>
+      <c r="BX10">
+        <f t="shared" si="6"/>
+        <v>184374.01616019674</v>
+      </c>
+      <c r="BY10">
+        <f t="shared" si="10"/>
+        <v>5.2656997158858312</v>
+      </c>
+      <c r="BZ10">
+        <v>718</v>
+      </c>
+      <c r="CA10">
+        <f>SUM(BV10:BZ10)</f>
+        <v>356065.28185991262</v>
       </c>
     </row>
     <row r="11" spans="1:79" x14ac:dyDescent="0.25">
@@ -5728,11 +5781,11 @@
         <v>1187552</v>
       </c>
       <c r="AV11" s="16">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>11048.371713407076</v>
       </c>
       <c r="AW11" s="16">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4.0432982772981152</v>
       </c>
       <c r="AX11" s="18">
@@ -5758,8 +5811,30 @@
       <c r="BE11" s="15"/>
       <c r="BK11" s="8"/>
       <c r="BT11" s="8"/>
-      <c r="BV11" t="s">
-        <v>23</v>
+      <c r="BU11" s="6">
+        <f t="shared" si="9"/>
+        <v>480878</v>
+      </c>
+      <c r="BV11">
+        <v>338172</v>
+      </c>
+      <c r="BW11">
+        <v>142706</v>
+      </c>
+      <c r="BX11">
+        <f t="shared" si="6"/>
+        <v>91940.884931257271</v>
+      </c>
+      <c r="BY11">
+        <f t="shared" si="10"/>
+        <v>4.9635086795199284</v>
+      </c>
+      <c r="BZ11">
+        <v>709</v>
+      </c>
+      <c r="CA11">
+        <f>SUM(BV11:BZ11)</f>
+        <v>573532.84843993676</v>
       </c>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.25">
@@ -5818,7 +5893,7 @@
         <v>287681</v>
       </c>
       <c r="AA12" s="17">
-        <f t="shared" ref="AA12" si="17">SUM(S12:T12,W12,Z12)</f>
+        <f t="shared" ref="AA12" si="18">SUM(S12:T12,W12,Z12)</f>
         <v>7230333</v>
       </c>
       <c r="AB12" s="15">
@@ -5832,7 +5907,7 @@
         <v>12879.988578294637</v>
       </c>
       <c r="AE12" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4.109915477900671</v>
       </c>
       <c r="AF12" s="15">
@@ -5850,7 +5925,7 @@
         <v>201019</v>
       </c>
       <c r="AJ12" s="8">
-        <f t="shared" ref="AJ12:AJ13" si="18">SUM(AI12,AF12,AC12,AB12)</f>
+        <f t="shared" ref="AJ12:AJ13" si="19">SUM(AI12,AF12,AC12,AB12)</f>
         <v>4234435</v>
       </c>
       <c r="AK12" s="18"/>
@@ -5869,11 +5944,11 @@
         <v>1426485</v>
       </c>
       <c r="AV12" s="16">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>18395.589052811632</v>
       </c>
       <c r="AW12" s="16">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4.2647136991141261</v>
       </c>
       <c r="AX12" s="18">
@@ -5961,7 +6036,7 @@
         <v>14188.329611566494</v>
       </c>
       <c r="AE13" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4.1519312690881582</v>
       </c>
       <c r="AF13" s="15">
@@ -5979,7 +6054,7 @@
         <v>199887</v>
       </c>
       <c r="AJ13" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8174345</v>
       </c>
       <c r="AS13" s="8"/>
@@ -5990,11 +6065,11 @@
         <v>1714057</v>
       </c>
       <c r="AV13" s="16">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>30618.622192844228</v>
       </c>
       <c r="AW13" s="16">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4.4859856439877221</v>
       </c>
       <c r="AX13">
@@ -6087,11 +6162,11 @@
         <v>3832440</v>
       </c>
       <c r="AV14" s="16">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>34235.411187128826</v>
       </c>
       <c r="AW14" s="16">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4.5344755483630772</v>
       </c>
       <c r="AX14">
@@ -6227,7 +6302,7 @@
         <v>143380</v>
       </c>
       <c r="C18" s="8">
-        <f t="shared" ref="C18:C26" si="19">LOG(B18)</f>
+        <f t="shared" ref="C18:C26" si="20">LOG(B18)</f>
         <v>5.156488576050017</v>
       </c>
       <c r="U18" s="15"/>
@@ -6255,7 +6330,7 @@
         <v>4550507</v>
       </c>
       <c r="C19" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>6.6580597867748397</v>
       </c>
       <c r="U19" s="15"/>
@@ -6283,7 +6358,7 @@
         <v>5927007</v>
       </c>
       <c r="C20" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>6.7728354401561059</v>
       </c>
       <c r="U20" s="15"/>
@@ -6311,7 +6386,7 @@
         <v>25820919</v>
       </c>
       <c r="C21" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7.4119716953094192</v>
       </c>
       <c r="U21" s="15"/>
@@ -6339,7 +6414,7 @@
         <v>838011150</v>
       </c>
       <c r="C22" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>8.9232497970923994</v>
       </c>
       <c r="U22" s="15"/>
@@ -6367,7 +6442,7 @@
         <v>2624103185</v>
       </c>
       <c r="C23" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.4189809083694165</v>
       </c>
       <c r="Z23" s="6"/>
@@ -6391,7 +6466,7 @@
         <v>4613302631</v>
       </c>
       <c r="C24" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.664011945105198</v>
       </c>
       <c r="Z24" s="6"/>
@@ -6415,7 +6490,7 @@
         <v>11538607113</v>
       </c>
       <c r="C25" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>10.062153385973239</v>
       </c>
       <c r="Z25" s="6"/>
@@ -6439,7 +6514,7 @@
         <v>23085163023</v>
       </c>
       <c r="C26" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>10.363332945802444</v>
       </c>
       <c r="Z26" s="6"/>
@@ -6495,7 +6570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>

</xml_diff>